<commit_message>
v0.4.2.1 alpha. Bugs fixed: Cid is not available in index when it is not shown.
</commit_message>
<xml_diff>
--- a/AIWE Table Making Guideline v20170926.xlsx
+++ b/AIWE Table Making Guideline v20170926.xlsx
@@ -18,15 +18,12 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="653" uniqueCount="542">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="656" uniqueCount="545">
   <si>
     <t>No</t>
   </si>
   <si>
     <t>Description</t>
-  </si>
-  <si>
-    <t>Every table must have a first column named Cid with data type of int as primary key and identity</t>
   </si>
   <si>
     <r>
@@ -2119,9 +2116,6 @@
   </si>
   <si>
     <t>NULL, --HistoryTrigger</t>
-  </si>
-  <si>
-    <t>NULL --AutoGeneratedColumns)</t>
   </si>
   <si>
     <t>insert into MetaItem values(</t>
@@ -2412,6 +2406,97 @@
         <scheme val="minor"/>
       </rPr>
       <t xml:space="preserve"> row action.</t>
+    </r>
+  </si>
+  <si>
+    <t>NULL, --AutoGeneratedColumns</t>
+  </si>
+  <si>
+    <t>NULL, --ColumnSequence</t>
+  </si>
+  <si>
+    <t>NULL, --ColumnAliases</t>
+  </si>
+  <si>
+    <t>NULL --EditShowOnlyColumns)</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Every table must have a first column named </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Cid</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> with data type of </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>int</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> as </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>primary key</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> and </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>identity</t>
     </r>
   </si>
 </sst>
@@ -2503,7 +2588,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="5">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -2525,6 +2610,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="6" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -2556,7 +2647,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="43">
+  <cellXfs count="44">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -2650,6 +2741,9 @@
     <xf numFmtId="0" fontId="7" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="7" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="7" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -2988,7 +3082,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:B42"/>
+  <dimension ref="A1:B45"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="B12" sqref="B12"/>
@@ -3002,7 +3096,7 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A1" s="3" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.3">
@@ -3018,13 +3112,13 @@
         <v>1</v>
       </c>
       <c r="B3" s="7" t="s">
-        <v>2</v>
+        <v>544</v>
       </c>
     </row>
     <row r="4" spans="1:2" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A4" s="6"/>
       <c r="B4" s="8" t="s">
-        <v>517</v>
+        <v>515</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.3">
@@ -3032,17 +3126,17 @@
         <v>2</v>
       </c>
       <c r="B5" s="7" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.3">
       <c r="B7" t="s">
-        <v>477</v>
+        <v>476</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.3">
       <c r="B8" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
     </row>
     <row r="9" spans="1:2" s="11" customFormat="1" x14ac:dyDescent="0.3">
@@ -3050,167 +3144,185 @@
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.3">
       <c r="B10" s="2" t="s">
-        <v>508</v>
+        <v>506</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.3">
       <c r="B11" s="17" t="s">
-        <v>509</v>
+        <v>507</v>
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.3">
       <c r="B12" s="17" t="s">
-        <v>510</v>
+        <v>508</v>
       </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.3">
       <c r="B13" t="s">
-        <v>478</v>
+        <v>477</v>
       </c>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.3">
       <c r="B14" t="s">
-        <v>479</v>
+        <v>478</v>
       </c>
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.3">
       <c r="B15" t="s">
-        <v>480</v>
+        <v>479</v>
       </c>
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.3">
       <c r="B16" t="s">
-        <v>481</v>
+        <v>480</v>
       </c>
     </row>
     <row r="17" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B17" t="s">
-        <v>482</v>
+        <v>481</v>
       </c>
     </row>
     <row r="18" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B18" t="s">
-        <v>483</v>
+        <v>482</v>
       </c>
     </row>
     <row r="19" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B19" t="s">
-        <v>484</v>
+        <v>483</v>
       </c>
     </row>
     <row r="20" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B20" t="s">
-        <v>485</v>
+        <v>484</v>
       </c>
     </row>
     <row r="21" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B21" t="s">
-        <v>486</v>
+        <v>485</v>
       </c>
     </row>
     <row r="22" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B22" t="s">
-        <v>487</v>
+        <v>486</v>
       </c>
     </row>
     <row r="23" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B23" t="s">
-        <v>488</v>
+        <v>487</v>
       </c>
     </row>
     <row r="24" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B24" t="s">
-        <v>489</v>
+        <v>488</v>
       </c>
     </row>
     <row r="25" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B25" t="s">
-        <v>490</v>
+        <v>489</v>
       </c>
     </row>
     <row r="26" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B26" t="s">
-        <v>491</v>
+        <v>490</v>
       </c>
     </row>
     <row r="27" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B27" t="s">
-        <v>492</v>
+        <v>491</v>
       </c>
     </row>
     <row r="28" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B28" t="s">
-        <v>493</v>
+        <v>492</v>
       </c>
     </row>
     <row r="29" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B29" t="s">
-        <v>494</v>
+        <v>493</v>
       </c>
     </row>
     <row r="30" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B30" t="s">
-        <v>495</v>
+        <v>494</v>
       </c>
     </row>
     <row r="31" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B31" t="s">
-        <v>496</v>
+        <v>495</v>
       </c>
     </row>
     <row r="32" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B32" t="s">
+        <v>496</v>
+      </c>
+    </row>
+    <row r="33" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="B33" t="s">
         <v>497</v>
       </c>
     </row>
-    <row r="33" spans="2:2" x14ac:dyDescent="0.3">
-      <c r="B33" t="s">
+    <row r="34" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="B34" t="s">
         <v>498</v>
       </c>
     </row>
-    <row r="34" spans="2:2" x14ac:dyDescent="0.3">
-      <c r="B34" t="s">
+    <row r="35" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="B35" t="s">
         <v>499</v>
       </c>
     </row>
-    <row r="35" spans="2:2" x14ac:dyDescent="0.3">
-      <c r="B35" t="s">
+    <row r="36" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="B36" t="s">
         <v>500</v>
       </c>
     </row>
-    <row r="36" spans="2:2" x14ac:dyDescent="0.3">
-      <c r="B36" t="s">
+    <row r="37" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="B37" t="s">
         <v>501</v>
       </c>
     </row>
-    <row r="37" spans="2:2" x14ac:dyDescent="0.3">
-      <c r="B37" t="s">
+    <row r="38" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="B38" t="s">
         <v>502</v>
       </c>
     </row>
-    <row r="38" spans="2:2" x14ac:dyDescent="0.3">
-      <c r="B38" t="s">
+    <row r="39" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="B39" t="s">
         <v>503</v>
       </c>
     </row>
-    <row r="39" spans="2:2" x14ac:dyDescent="0.3">
-      <c r="B39" t="s">
+    <row r="40" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="B40" t="s">
         <v>504</v>
       </c>
     </row>
-    <row r="40" spans="2:2" x14ac:dyDescent="0.3">
-      <c r="B40" t="s">
+    <row r="41" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="B41" t="s">
         <v>505</v>
       </c>
     </row>
-    <row r="41" spans="2:2" x14ac:dyDescent="0.3">
-      <c r="B41" t="s">
-        <v>506</v>
-      </c>
-    </row>
-    <row r="42" spans="2:2" x14ac:dyDescent="0.3">
-      <c r="B42" t="s">
-        <v>507</v>
+    <row r="42" spans="1:2" s="11" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A42" s="1"/>
+      <c r="B42" s="11" t="s">
+        <v>540</v>
+      </c>
+    </row>
+    <row r="43" spans="1:2" s="11" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A43" s="1"/>
+      <c r="B43" s="11" t="s">
+        <v>541</v>
+      </c>
+    </row>
+    <row r="44" spans="1:2" s="11" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A44" s="1"/>
+      <c r="B44" s="11" t="s">
+        <v>542</v>
+      </c>
+    </row>
+    <row r="45" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="B45" t="s">
+        <v>543</v>
       </c>
     </row>
   </sheetData>
@@ -3223,8 +3335,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:E44"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A37" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C49" sqref="C49"/>
+    <sheetView tabSelected="1" topLeftCell="C30" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="D30" sqref="D30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -3239,7 +3351,7 @@
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A1" s="18" t="s">
-        <v>518</v>
+        <v>516</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.3">
@@ -3247,16 +3359,16 @@
         <v>0</v>
       </c>
       <c r="B2" s="22" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C2" s="22" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="D2" s="23" t="s">
         <v>1</v>
       </c>
       <c r="E2" s="24" t="s">
-        <v>313</v>
+        <v>312</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.3">
@@ -3264,13 +3376,13 @@
         <v>1</v>
       </c>
       <c r="B3" s="26" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C3" s="26" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="D3" s="27" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="E3" s="28"/>
     </row>
@@ -3279,13 +3391,13 @@
         <v>2</v>
       </c>
       <c r="B4" s="27" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="C4" s="27" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="D4" s="27" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="E4" s="28"/>
     </row>
@@ -3294,13 +3406,13 @@
         <v>3</v>
       </c>
       <c r="B5" s="26" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="C5" s="26" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="D5" s="27" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="E5" s="28"/>
     </row>
@@ -3309,13 +3421,13 @@
         <v>4</v>
       </c>
       <c r="B6" s="26" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="C6" s="27" t="s">
+        <v>140</v>
+      </c>
+      <c r="D6" s="30" t="s">
         <v>141</v>
-      </c>
-      <c r="D6" s="30" t="s">
-        <v>142</v>
       </c>
       <c r="E6" s="28"/>
     </row>
@@ -3324,13 +3436,13 @@
         <v>5</v>
       </c>
       <c r="B7" s="26" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C7" s="27" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="D7" s="30" t="s">
-        <v>519</v>
+        <v>517</v>
       </c>
       <c r="E7" s="28"/>
     </row>
@@ -3339,13 +3451,13 @@
         <v>6</v>
       </c>
       <c r="B8" s="31" t="s">
-        <v>511</v>
+        <v>509</v>
       </c>
       <c r="C8" s="27" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="D8" s="27" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="E8" s="28"/>
     </row>
@@ -3354,13 +3466,13 @@
         <v>7</v>
       </c>
       <c r="B9" s="26" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="C9" s="27" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="D9" s="30" t="s">
-        <v>520</v>
+        <v>518</v>
       </c>
       <c r="E9" s="28"/>
     </row>
@@ -3369,13 +3481,13 @@
         <v>8</v>
       </c>
       <c r="B10" s="31" t="s">
-        <v>512</v>
+        <v>510</v>
       </c>
       <c r="C10" s="26" t="s">
+        <v>29</v>
+      </c>
+      <c r="D10" s="27" t="s">
         <v>30</v>
-      </c>
-      <c r="D10" s="27" t="s">
-        <v>31</v>
       </c>
       <c r="E10" s="28"/>
     </row>
@@ -3384,13 +3496,13 @@
         <v>9</v>
       </c>
       <c r="B11" s="31" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="C11" s="27" t="s">
+        <v>127</v>
+      </c>
+      <c r="D11" s="30" t="s">
         <v>128</v>
-      </c>
-      <c r="D11" s="30" t="s">
-        <v>129</v>
       </c>
       <c r="E11" s="28"/>
     </row>
@@ -3399,13 +3511,13 @@
         <v>10</v>
       </c>
       <c r="B12" s="31" t="s">
-        <v>513</v>
+        <v>511</v>
       </c>
       <c r="C12" s="27" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="D12" s="30" t="s">
-        <v>521</v>
+        <v>519</v>
       </c>
       <c r="E12" s="28"/>
     </row>
@@ -3414,13 +3526,13 @@
         <v>11</v>
       </c>
       <c r="B13" s="27" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="C13" s="27" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="D13" s="30" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="E13" s="28"/>
     </row>
@@ -3429,13 +3541,13 @@
         <v>12</v>
       </c>
       <c r="B14" s="26" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="C14" s="26" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="D14" s="30" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="E14" s="28"/>
     </row>
@@ -3444,13 +3556,13 @@
         <v>13</v>
       </c>
       <c r="B15" s="31" t="s">
-        <v>514</v>
+        <v>512</v>
       </c>
       <c r="C15" s="32" t="s">
-        <v>476</v>
+        <v>475</v>
       </c>
       <c r="D15" s="30" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="E15" s="28"/>
     </row>
@@ -3459,13 +3571,13 @@
         <v>14</v>
       </c>
       <c r="B16" s="27" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="C16" s="30" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="D16" s="32" t="s">
-        <v>522</v>
+        <v>520</v>
       </c>
       <c r="E16" s="28"/>
     </row>
@@ -3474,13 +3586,13 @@
         <v>15</v>
       </c>
       <c r="B17" s="27" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="C17" s="30" t="s">
+        <v>44</v>
+      </c>
+      <c r="D17" s="30" t="s">
         <v>45</v>
-      </c>
-      <c r="D17" s="30" t="s">
-        <v>46</v>
       </c>
       <c r="E17" s="28"/>
     </row>
@@ -3489,16 +3601,16 @@
         <v>16</v>
       </c>
       <c r="B18" s="27" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="C18" s="30" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="D18" s="30" t="s">
-        <v>523</v>
+        <v>521</v>
       </c>
       <c r="E18" s="33" t="s">
-        <v>312</v>
+        <v>311</v>
       </c>
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.3">
@@ -3506,13 +3618,13 @@
         <v>17</v>
       </c>
       <c r="B19" s="26" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C19" s="27" t="s">
+        <v>22</v>
+      </c>
+      <c r="D19" s="27" t="s">
         <v>23</v>
-      </c>
-      <c r="D19" s="27" t="s">
-        <v>24</v>
       </c>
       <c r="E19" s="28"/>
     </row>
@@ -3521,13 +3633,13 @@
         <v>18</v>
       </c>
       <c r="B20" s="26" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C20" s="27" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="D20" s="30" t="s">
-        <v>524</v>
+        <v>522</v>
       </c>
       <c r="E20" s="28"/>
     </row>
@@ -3536,13 +3648,13 @@
         <v>19</v>
       </c>
       <c r="B21" s="26" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C21" s="27" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="D21" s="30" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="E21" s="28"/>
     </row>
@@ -3551,13 +3663,13 @@
         <v>20</v>
       </c>
       <c r="B22" s="26" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="C22" s="27" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="D22" s="30" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="E22" s="28"/>
     </row>
@@ -3566,13 +3678,13 @@
         <v>21</v>
       </c>
       <c r="B23" s="26" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C23" s="27" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="D23" s="30" t="s">
-        <v>525</v>
+        <v>523</v>
       </c>
       <c r="E23" s="28"/>
     </row>
@@ -3581,13 +3693,13 @@
         <v>22</v>
       </c>
       <c r="B24" s="26" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C24" s="27" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="D24" s="34" t="s">
-        <v>526</v>
+        <v>524</v>
       </c>
       <c r="E24" s="28"/>
     </row>
@@ -3596,16 +3708,16 @@
         <v>23</v>
       </c>
       <c r="B25" s="31" t="s">
-        <v>515</v>
+        <v>513</v>
       </c>
       <c r="C25" s="26" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="D25" s="30" t="s">
-        <v>527</v>
+        <v>525</v>
       </c>
       <c r="E25" s="33" t="s">
-        <v>314</v>
+        <v>313</v>
       </c>
     </row>
     <row r="26" spans="1:5" ht="86.4" x14ac:dyDescent="0.3">
@@ -3613,16 +3725,16 @@
         <v>24</v>
       </c>
       <c r="B26" s="26" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C26" s="35" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="D26" s="30" t="s">
-        <v>528</v>
+        <v>526</v>
       </c>
       <c r="E26" s="28" t="s">
-        <v>315</v>
+        <v>314</v>
       </c>
     </row>
     <row r="27" spans="1:5" ht="115.2" x14ac:dyDescent="0.3">
@@ -3630,16 +3742,16 @@
         <v>25</v>
       </c>
       <c r="B27" s="26" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="C27" s="30" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="D27" s="30" t="s">
-        <v>529</v>
+        <v>527</v>
       </c>
       <c r="E27" s="33" t="s">
-        <v>316</v>
+        <v>315</v>
       </c>
     </row>
     <row r="28" spans="1:5" s="19" customFormat="1" x14ac:dyDescent="0.3">
@@ -3647,13 +3759,13 @@
         <v>26</v>
       </c>
       <c r="B28" s="27" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="C28" s="27" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="D28" s="27" t="s">
-        <v>540</v>
+        <v>538</v>
       </c>
       <c r="E28" s="28"/>
     </row>
@@ -3662,13 +3774,13 @@
         <v>27</v>
       </c>
       <c r="B29" s="27" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="C29" s="27" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="D29" s="27" t="s">
-        <v>541</v>
+        <v>539</v>
       </c>
       <c r="E29" s="28"/>
     </row>
@@ -3677,16 +3789,16 @@
         <v>28</v>
       </c>
       <c r="B30" s="27" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="C30" s="30" t="s">
-        <v>189</v>
-      </c>
-      <c r="D30" s="30" t="s">
-        <v>530</v>
+        <v>188</v>
+      </c>
+      <c r="D30" s="43" t="s">
+        <v>528</v>
       </c>
       <c r="E30" s="33" t="s">
-        <v>317</v>
+        <v>316</v>
       </c>
     </row>
     <row r="31" spans="1:5" s="19" customFormat="1" ht="158.4" x14ac:dyDescent="0.3">
@@ -3694,16 +3806,16 @@
         <v>29</v>
       </c>
       <c r="B31" s="27" t="s">
-        <v>516</v>
+        <v>514</v>
       </c>
       <c r="C31" s="30" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="D31" s="30" t="s">
-        <v>531</v>
+        <v>529</v>
       </c>
       <c r="E31" s="33" t="s">
-        <v>318</v>
+        <v>317</v>
       </c>
     </row>
     <row r="32" spans="1:5" s="19" customFormat="1" x14ac:dyDescent="0.3">
@@ -3711,13 +3823,13 @@
         <v>30</v>
       </c>
       <c r="B32" s="27" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="C32" s="30" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="D32" s="30" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="E32" s="28"/>
     </row>
@@ -3726,13 +3838,13 @@
         <v>31</v>
       </c>
       <c r="B33" s="27" t="s">
+        <v>170</v>
+      </c>
+      <c r="C33" s="30" t="s">
         <v>171</v>
       </c>
-      <c r="C33" s="30" t="s">
-        <v>172</v>
-      </c>
       <c r="D33" s="30" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="E33" s="28"/>
     </row>
@@ -3741,16 +3853,16 @@
         <v>32</v>
       </c>
       <c r="B34" s="27" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="C34" s="30" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="D34" s="30" t="s">
-        <v>532</v>
+        <v>530</v>
       </c>
       <c r="E34" s="33" t="s">
-        <v>319</v>
+        <v>318</v>
       </c>
     </row>
     <row r="35" spans="1:5" s="40" customFormat="1" ht="57.6" x14ac:dyDescent="0.3">
@@ -3758,13 +3870,13 @@
         <v>33</v>
       </c>
       <c r="B35" s="37" t="s">
-        <v>533</v>
+        <v>531</v>
       </c>
       <c r="C35" s="38" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="D35" s="38" t="s">
-        <v>536</v>
+        <v>534</v>
       </c>
       <c r="E35" s="39"/>
     </row>
@@ -3773,13 +3885,13 @@
         <v>34</v>
       </c>
       <c r="B36" s="37" t="s">
-        <v>534</v>
+        <v>532</v>
       </c>
       <c r="C36" s="38" t="s">
+        <v>533</v>
+      </c>
+      <c r="D36" s="38" t="s">
         <v>535</v>
-      </c>
-      <c r="D36" s="38" t="s">
-        <v>537</v>
       </c>
       <c r="E36" s="39"/>
     </row>
@@ -3788,39 +3900,39 @@
         <v>35</v>
       </c>
       <c r="B37" s="37" t="s">
-        <v>538</v>
+        <v>536</v>
       </c>
       <c r="C37" s="38" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="D37" s="38" t="s">
-        <v>539</v>
+        <v>537</v>
       </c>
       <c r="E37" s="39"/>
     </row>
     <row r="40" spans="1:5" x14ac:dyDescent="0.3">
       <c r="B40" s="41" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
     </row>
     <row r="41" spans="1:5" x14ac:dyDescent="0.3">
       <c r="B41" s="26" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
     </row>
     <row r="42" spans="1:5" x14ac:dyDescent="0.3">
       <c r="B42" s="37" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
     </row>
     <row r="43" spans="1:5" x14ac:dyDescent="0.3">
       <c r="B43" s="31" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
     </row>
     <row r="44" spans="1:5" x14ac:dyDescent="0.3">
       <c r="B44" s="42" t="s">
-        <v>311</v>
+        <v>310</v>
       </c>
     </row>
   </sheetData>
@@ -3846,7 +3958,7 @@
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.3">
@@ -3854,13 +3966,13 @@
         <v>0</v>
       </c>
       <c r="B2" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="C2" t="s">
         <v>1</v>
       </c>
       <c r="D2" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.3">
@@ -3868,13 +3980,13 @@
         <v>1</v>
       </c>
       <c r="B3" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="C3" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
       <c r="D3" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.3">
@@ -3882,13 +3994,13 @@
         <v>2</v>
       </c>
       <c r="B4" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="C4" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="D4" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
     </row>
   </sheetData>
@@ -3914,23 +4026,23 @@
   <sheetData>
     <row r="1" spans="1:3" s="11" customFormat="1" ht="18" x14ac:dyDescent="0.35">
       <c r="A1" s="16" t="s">
-        <v>475</v>
+        <v>474</v>
       </c>
     </row>
     <row r="2" spans="1:3" s="11" customFormat="1" ht="18" x14ac:dyDescent="0.35">
       <c r="A2" s="16" t="s">
-        <v>474</v>
+        <v>473</v>
       </c>
     </row>
     <row r="3" spans="1:3" s="11" customFormat="1" x14ac:dyDescent="0.3"/>
     <row r="4" spans="1:3" s="11" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A4" s="11" t="s">
-        <v>470</v>
+        <v>469</v>
       </c>
     </row>
     <row r="5" spans="1:3" s="11" customFormat="1" x14ac:dyDescent="0.3">
       <c r="B5" s="11" t="s">
-        <v>455</v>
+        <v>454</v>
       </c>
     </row>
     <row r="6" spans="1:3" s="11" customFormat="1" x14ac:dyDescent="0.3">
@@ -3938,13 +4050,13 @@
         <v>1</v>
       </c>
       <c r="C6" s="11" t="s">
-        <v>471</v>
+        <v>470</v>
       </c>
     </row>
     <row r="7" spans="1:3" s="11" customFormat="1" x14ac:dyDescent="0.3"/>
     <row r="8" spans="1:3" s="11" customFormat="1" x14ac:dyDescent="0.3">
       <c r="B8" s="11" t="s">
-        <v>466</v>
+        <v>465</v>
       </c>
     </row>
     <row r="9" spans="1:3" s="11" customFormat="1" x14ac:dyDescent="0.3">
@@ -3952,7 +4064,7 @@
         <v>1</v>
       </c>
       <c r="C9" s="11" t="s">
-        <v>472</v>
+        <v>471</v>
       </c>
     </row>
     <row r="10" spans="1:3" s="11" customFormat="1" x14ac:dyDescent="0.3">
@@ -3960,18 +4072,18 @@
         <v>2</v>
       </c>
       <c r="C10" s="11" t="s">
-        <v>473</v>
+        <v>472</v>
       </c>
     </row>
     <row r="11" spans="1:3" s="11" customFormat="1" x14ac:dyDescent="0.3"/>
     <row r="12" spans="1:3" s="11" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A12" s="11" t="s">
-        <v>468</v>
+        <v>467</v>
       </c>
     </row>
     <row r="13" spans="1:3" s="11" customFormat="1" x14ac:dyDescent="0.3">
       <c r="B13" s="11" t="s">
-        <v>455</v>
+        <v>454</v>
       </c>
     </row>
     <row r="14" spans="1:3" s="11" customFormat="1" x14ac:dyDescent="0.3">
@@ -3979,18 +4091,18 @@
         <v>1</v>
       </c>
       <c r="C14" s="11" t="s">
-        <v>469</v>
+        <v>468</v>
       </c>
     </row>
     <row r="15" spans="1:3" s="11" customFormat="1" x14ac:dyDescent="0.3"/>
     <row r="16" spans="1:3" s="11" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A16" s="11" t="s">
-        <v>462</v>
+        <v>461</v>
       </c>
     </row>
     <row r="17" spans="1:3" s="11" customFormat="1" x14ac:dyDescent="0.3">
       <c r="B17" s="11" t="s">
-        <v>455</v>
+        <v>454</v>
       </c>
     </row>
     <row r="18" spans="1:3" s="11" customFormat="1" x14ac:dyDescent="0.3">
@@ -3998,7 +4110,7 @@
         <v>1</v>
       </c>
       <c r="C18" s="11" t="s">
-        <v>463</v>
+        <v>462</v>
       </c>
     </row>
     <row r="19" spans="1:3" s="11" customFormat="1" x14ac:dyDescent="0.3">
@@ -4006,7 +4118,7 @@
         <v>2</v>
       </c>
       <c r="C19" s="11" t="s">
-        <v>464</v>
+        <v>463</v>
       </c>
     </row>
     <row r="20" spans="1:3" s="11" customFormat="1" x14ac:dyDescent="0.3">
@@ -4014,13 +4126,13 @@
         <v>3</v>
       </c>
       <c r="C20" s="11" t="s">
-        <v>465</v>
+        <v>464</v>
       </c>
     </row>
     <row r="21" spans="1:3" s="11" customFormat="1" x14ac:dyDescent="0.3"/>
     <row r="22" spans="1:3" s="11" customFormat="1" x14ac:dyDescent="0.3">
       <c r="B22" s="11" t="s">
-        <v>466</v>
+        <v>465</v>
       </c>
     </row>
     <row r="23" spans="1:3" s="11" customFormat="1" x14ac:dyDescent="0.3">
@@ -4028,18 +4140,18 @@
         <v>1</v>
       </c>
       <c r="C23" s="11" t="s">
-        <v>467</v>
+        <v>466</v>
       </c>
     </row>
     <row r="24" spans="1:3" s="11" customFormat="1" x14ac:dyDescent="0.3"/>
     <row r="25" spans="1:3" s="11" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A25" s="11" t="s">
-        <v>453</v>
+        <v>452</v>
       </c>
     </row>
     <row r="26" spans="1:3" s="11" customFormat="1" x14ac:dyDescent="0.3">
       <c r="B26" s="11" t="s">
-        <v>455</v>
+        <v>454</v>
       </c>
     </row>
     <row r="27" spans="1:3" s="11" customFormat="1" x14ac:dyDescent="0.3">
@@ -4047,7 +4159,7 @@
         <v>1</v>
       </c>
       <c r="C27" s="11" t="s">
-        <v>454</v>
+        <v>453</v>
       </c>
     </row>
     <row r="28" spans="1:3" s="11" customFormat="1" x14ac:dyDescent="0.3">
@@ -4055,7 +4167,7 @@
         <v>2</v>
       </c>
       <c r="C28" s="11" t="s">
-        <v>458</v>
+        <v>457</v>
       </c>
     </row>
     <row r="29" spans="1:3" s="11" customFormat="1" x14ac:dyDescent="0.3">
@@ -4063,7 +4175,7 @@
         <v>3</v>
       </c>
       <c r="C29" s="11" t="s">
-        <v>459</v>
+        <v>458</v>
       </c>
     </row>
     <row r="30" spans="1:3" s="11" customFormat="1" x14ac:dyDescent="0.3">
@@ -4071,7 +4183,7 @@
         <v>4</v>
       </c>
       <c r="C30" s="11" t="s">
-        <v>460</v>
+        <v>459</v>
       </c>
     </row>
     <row r="31" spans="1:3" s="11" customFormat="1" x14ac:dyDescent="0.3">
@@ -4079,7 +4191,7 @@
         <v>5</v>
       </c>
       <c r="C31" s="11" t="s">
-        <v>456</v>
+        <v>455</v>
       </c>
     </row>
     <row r="32" spans="1:3" s="11" customFormat="1" x14ac:dyDescent="0.3">
@@ -4087,7 +4199,7 @@
         <v>6</v>
       </c>
       <c r="C32" s="11" t="s">
-        <v>457</v>
+        <v>456</v>
       </c>
     </row>
     <row r="33" spans="1:3" s="11" customFormat="1" x14ac:dyDescent="0.3">
@@ -4095,18 +4207,18 @@
         <v>7</v>
       </c>
       <c r="C33" s="11" t="s">
-        <v>461</v>
+        <v>460</v>
       </c>
     </row>
     <row r="34" spans="1:3" s="11" customFormat="1" x14ac:dyDescent="0.3"/>
     <row r="35" spans="1:3" s="11" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A35" s="11" t="s">
-        <v>452</v>
+        <v>451</v>
       </c>
     </row>
     <row r="36" spans="1:3" s="11" customFormat="1" x14ac:dyDescent="0.3">
       <c r="B36" s="11" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
     </row>
     <row r="37" spans="1:3" s="11" customFormat="1" x14ac:dyDescent="0.3">
@@ -4114,7 +4226,7 @@
         <v>1</v>
       </c>
       <c r="C37" s="11" t="s">
-        <v>449</v>
+        <v>448</v>
       </c>
     </row>
     <row r="38" spans="1:3" s="11" customFormat="1" x14ac:dyDescent="0.3">
@@ -4122,7 +4234,7 @@
         <v>2</v>
       </c>
       <c r="C38" s="11" t="s">
-        <v>450</v>
+        <v>449</v>
       </c>
     </row>
     <row r="39" spans="1:3" s="11" customFormat="1" x14ac:dyDescent="0.3">
@@ -4130,18 +4242,18 @@
         <v>3</v>
       </c>
       <c r="C39" s="11" t="s">
-        <v>451</v>
+        <v>450</v>
       </c>
     </row>
     <row r="40" spans="1:3" s="11" customFormat="1" x14ac:dyDescent="0.3"/>
     <row r="41" spans="1:3" s="11" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A41" s="11" t="s">
-        <v>432</v>
+        <v>431</v>
       </c>
     </row>
     <row r="42" spans="1:3" s="11" customFormat="1" x14ac:dyDescent="0.3">
       <c r="B42" s="11" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
     </row>
     <row r="43" spans="1:3" s="11" customFormat="1" x14ac:dyDescent="0.3">
@@ -4149,12 +4261,12 @@
         <v>1</v>
       </c>
       <c r="C43" s="11" t="s">
-        <v>433</v>
+        <v>432</v>
       </c>
     </row>
     <row r="44" spans="1:3" s="11" customFormat="1" x14ac:dyDescent="0.3">
       <c r="B44" s="11" t="s">
-        <v>402</v>
+        <v>401</v>
       </c>
     </row>
     <row r="45" spans="1:3" s="11" customFormat="1" x14ac:dyDescent="0.3">
@@ -4162,12 +4274,12 @@
         <v>1</v>
       </c>
       <c r="C45" s="11" t="s">
-        <v>434</v>
+        <v>433</v>
       </c>
     </row>
     <row r="46" spans="1:3" s="11" customFormat="1" x14ac:dyDescent="0.3">
       <c r="C46" s="11" t="s">
-        <v>435</v>
+        <v>434</v>
       </c>
     </row>
     <row r="47" spans="1:3" s="11" customFormat="1" x14ac:dyDescent="0.3">
@@ -4175,12 +4287,12 @@
         <v>2</v>
       </c>
       <c r="C47" s="11" t="s">
-        <v>437</v>
+        <v>436</v>
       </c>
     </row>
     <row r="48" spans="1:3" s="11" customFormat="1" x14ac:dyDescent="0.3">
       <c r="C48" s="11" t="s">
-        <v>436</v>
+        <v>435</v>
       </c>
     </row>
     <row r="49" spans="1:3" s="11" customFormat="1" x14ac:dyDescent="0.3">
@@ -4188,12 +4300,12 @@
         <v>3</v>
       </c>
       <c r="C49" s="11" t="s">
-        <v>448</v>
+        <v>447</v>
       </c>
     </row>
     <row r="50" spans="1:3" s="11" customFormat="1" x14ac:dyDescent="0.3">
       <c r="B50" s="11" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
     </row>
     <row r="51" spans="1:3" s="11" customFormat="1" x14ac:dyDescent="0.3">
@@ -4201,7 +4313,7 @@
         <v>1</v>
       </c>
       <c r="C51" s="11" t="s">
-        <v>442</v>
+        <v>441</v>
       </c>
     </row>
     <row r="52" spans="1:3" s="11" customFormat="1" x14ac:dyDescent="0.3">
@@ -4209,7 +4321,7 @@
         <v>2</v>
       </c>
       <c r="C52" s="11" t="s">
-        <v>447</v>
+        <v>446</v>
       </c>
     </row>
     <row r="53" spans="1:3" s="11" customFormat="1" x14ac:dyDescent="0.3">
@@ -4217,7 +4329,7 @@
         <v>3</v>
       </c>
       <c r="C53" s="11" t="s">
-        <v>441</v>
+        <v>440</v>
       </c>
     </row>
     <row r="54" spans="1:3" s="11" customFormat="1" x14ac:dyDescent="0.3">
@@ -4225,7 +4337,7 @@
         <v>4</v>
       </c>
       <c r="C54" s="11" t="s">
-        <v>440</v>
+        <v>439</v>
       </c>
     </row>
     <row r="55" spans="1:3" s="11" customFormat="1" x14ac:dyDescent="0.3">
@@ -4233,7 +4345,7 @@
         <v>5</v>
       </c>
       <c r="C55" s="11" t="s">
-        <v>433</v>
+        <v>432</v>
       </c>
     </row>
     <row r="56" spans="1:3" s="11" customFormat="1" x14ac:dyDescent="0.3">
@@ -4241,7 +4353,7 @@
         <v>6</v>
       </c>
       <c r="C56" s="11" t="s">
-        <v>438</v>
+        <v>437</v>
       </c>
     </row>
     <row r="57" spans="1:3" s="11" customFormat="1" x14ac:dyDescent="0.3">
@@ -4249,7 +4361,7 @@
         <v>7</v>
       </c>
       <c r="C57" s="11" t="s">
-        <v>439</v>
+        <v>438</v>
       </c>
     </row>
     <row r="58" spans="1:3" s="11" customFormat="1" x14ac:dyDescent="0.3">
@@ -4257,7 +4369,7 @@
         <v>8</v>
       </c>
       <c r="C58" s="11" t="s">
-        <v>446</v>
+        <v>445</v>
       </c>
     </row>
     <row r="59" spans="1:3" s="11" customFormat="1" x14ac:dyDescent="0.3">
@@ -4265,7 +4377,7 @@
         <v>9</v>
       </c>
       <c r="C59" s="11" t="s">
-        <v>443</v>
+        <v>442</v>
       </c>
     </row>
     <row r="60" spans="1:3" s="11" customFormat="1" x14ac:dyDescent="0.3">
@@ -4273,7 +4385,7 @@
         <v>10</v>
       </c>
       <c r="C60" s="11" t="s">
-        <v>444</v>
+        <v>443</v>
       </c>
     </row>
     <row r="61" spans="1:3" s="11" customFormat="1" x14ac:dyDescent="0.3">
@@ -4281,18 +4393,18 @@
         <v>11</v>
       </c>
       <c r="C61" s="11" t="s">
-        <v>445</v>
+        <v>444</v>
       </c>
     </row>
     <row r="62" spans="1:3" s="11" customFormat="1" x14ac:dyDescent="0.3"/>
     <row r="63" spans="1:3" s="11" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A63" s="11" t="s">
-        <v>422</v>
+        <v>421</v>
       </c>
     </row>
     <row r="64" spans="1:3" s="11" customFormat="1" x14ac:dyDescent="0.3">
       <c r="B64" s="11" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
     </row>
     <row r="65" spans="1:3" s="11" customFormat="1" x14ac:dyDescent="0.3">
@@ -4300,7 +4412,7 @@
         <v>1</v>
       </c>
       <c r="C65" s="14" t="s">
-        <v>429</v>
+        <v>428</v>
       </c>
     </row>
     <row r="66" spans="1:3" s="11" customFormat="1" x14ac:dyDescent="0.3">
@@ -4308,7 +4420,7 @@
         <v>2</v>
       </c>
       <c r="C66" s="11" t="s">
-        <v>430</v>
+        <v>429</v>
       </c>
     </row>
     <row r="67" spans="1:3" s="11" customFormat="1" x14ac:dyDescent="0.3">
@@ -4316,27 +4428,27 @@
         <v>3</v>
       </c>
       <c r="C67" s="11" t="s">
-        <v>423</v>
+        <v>422</v>
       </c>
     </row>
     <row r="68" spans="1:3" s="11" customFormat="1" x14ac:dyDescent="0.3">
       <c r="C68" s="11" t="s">
-        <v>425</v>
+        <v>424</v>
       </c>
     </row>
     <row r="69" spans="1:3" s="11" customFormat="1" x14ac:dyDescent="0.3">
       <c r="C69" s="11" t="s">
-        <v>426</v>
+        <v>425</v>
       </c>
     </row>
     <row r="70" spans="1:3" s="11" customFormat="1" x14ac:dyDescent="0.3">
       <c r="C70" s="11" t="s">
-        <v>427</v>
+        <v>426</v>
       </c>
     </row>
     <row r="71" spans="1:3" s="11" customFormat="1" x14ac:dyDescent="0.3">
       <c r="C71" s="11" t="s">
-        <v>428</v>
+        <v>427</v>
       </c>
     </row>
     <row r="72" spans="1:3" s="11" customFormat="1" x14ac:dyDescent="0.3">
@@ -4344,7 +4456,7 @@
         <v>4</v>
       </c>
       <c r="C72" s="11" t="s">
-        <v>424</v>
+        <v>423</v>
       </c>
     </row>
     <row r="73" spans="1:3" s="11" customFormat="1" x14ac:dyDescent="0.3">
@@ -4352,18 +4464,18 @@
         <v>5</v>
       </c>
       <c r="C73" s="11" t="s">
-        <v>431</v>
+        <v>430</v>
       </c>
     </row>
     <row r="74" spans="1:3" s="11" customFormat="1" x14ac:dyDescent="0.3"/>
     <row r="75" spans="1:3" s="11" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A75" s="11" t="s">
-        <v>411</v>
+        <v>410</v>
       </c>
     </row>
     <row r="76" spans="1:3" s="11" customFormat="1" x14ac:dyDescent="0.3">
       <c r="B76" s="11" t="s">
-        <v>402</v>
+        <v>401</v>
       </c>
     </row>
     <row r="77" spans="1:3" s="11" customFormat="1" x14ac:dyDescent="0.3">
@@ -4371,12 +4483,12 @@
         <v>1</v>
       </c>
       <c r="C77" s="11" t="s">
-        <v>412</v>
+        <v>411</v>
       </c>
     </row>
     <row r="78" spans="1:3" s="11" customFormat="1" x14ac:dyDescent="0.3">
       <c r="C78" s="11" t="s">
-        <v>414</v>
+        <v>413</v>
       </c>
     </row>
     <row r="79" spans="1:3" s="11" customFormat="1" x14ac:dyDescent="0.3">
@@ -4384,17 +4496,17 @@
         <v>2</v>
       </c>
       <c r="C79" s="11" t="s">
-        <v>413</v>
+        <v>412</v>
       </c>
     </row>
     <row r="80" spans="1:3" s="11" customFormat="1" x14ac:dyDescent="0.3">
       <c r="C80" s="11" t="s">
-        <v>415</v>
+        <v>414</v>
       </c>
     </row>
     <row r="81" spans="1:3" s="11" customFormat="1" x14ac:dyDescent="0.3">
       <c r="C81" s="11" t="s">
-        <v>416</v>
+        <v>415</v>
       </c>
     </row>
     <row r="82" spans="1:3" s="11" customFormat="1" x14ac:dyDescent="0.3">
@@ -4402,22 +4514,22 @@
         <v>3</v>
       </c>
       <c r="C82" s="11" t="s">
-        <v>417</v>
+        <v>416</v>
       </c>
     </row>
     <row r="83" spans="1:3" s="11" customFormat="1" x14ac:dyDescent="0.3">
       <c r="C83" s="11" t="s">
-        <v>418</v>
+        <v>417</v>
       </c>
     </row>
     <row r="84" spans="1:3" s="11" customFormat="1" x14ac:dyDescent="0.3">
       <c r="C84" s="11" t="s">
-        <v>419</v>
+        <v>418</v>
       </c>
     </row>
     <row r="85" spans="1:3" s="11" customFormat="1" x14ac:dyDescent="0.3">
       <c r="B85" s="11" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
     </row>
     <row r="86" spans="1:3" s="11" customFormat="1" x14ac:dyDescent="0.3">
@@ -4425,7 +4537,7 @@
         <v>1</v>
       </c>
       <c r="C86" s="11" t="s">
-        <v>420</v>
+        <v>419</v>
       </c>
     </row>
     <row r="87" spans="1:3" s="11" customFormat="1" x14ac:dyDescent="0.3">
@@ -4433,18 +4545,18 @@
         <v>2</v>
       </c>
       <c r="C87" s="11" t="s">
-        <v>421</v>
+        <v>420</v>
       </c>
     </row>
     <row r="88" spans="1:3" s="11" customFormat="1" x14ac:dyDescent="0.3"/>
     <row r="89" spans="1:3" s="11" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A89" s="11" t="s">
-        <v>400</v>
+        <v>399</v>
       </c>
     </row>
     <row r="90" spans="1:3" s="11" customFormat="1" x14ac:dyDescent="0.3">
       <c r="B90" s="11" t="s">
-        <v>401</v>
+        <v>400</v>
       </c>
     </row>
     <row r="91" spans="1:3" s="11" customFormat="1" x14ac:dyDescent="0.3">
@@ -4452,12 +4564,12 @@
         <v>1</v>
       </c>
       <c r="C91" s="11" t="s">
-        <v>405</v>
+        <v>404</v>
       </c>
     </row>
     <row r="92" spans="1:3" s="11" customFormat="1" x14ac:dyDescent="0.3">
       <c r="B92" s="11" t="s">
-        <v>402</v>
+        <v>401</v>
       </c>
     </row>
     <row r="93" spans="1:3" s="11" customFormat="1" x14ac:dyDescent="0.3">
@@ -4465,7 +4577,7 @@
         <v>1</v>
       </c>
       <c r="C93" s="11" t="s">
-        <v>405</v>
+        <v>404</v>
       </c>
     </row>
     <row r="94" spans="1:3" s="11" customFormat="1" x14ac:dyDescent="0.3">
@@ -4473,7 +4585,7 @@
         <v>2</v>
       </c>
       <c r="C94" s="11" t="s">
-        <v>403</v>
+        <v>402</v>
       </c>
     </row>
     <row r="95" spans="1:3" s="11" customFormat="1" x14ac:dyDescent="0.3">
@@ -4481,12 +4593,12 @@
         <v>3</v>
       </c>
       <c r="C95" s="11" t="s">
-        <v>404</v>
+        <v>403</v>
       </c>
     </row>
     <row r="96" spans="1:3" s="11" customFormat="1" x14ac:dyDescent="0.3">
       <c r="B96" s="11" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
     </row>
     <row r="97" spans="1:3" s="11" customFormat="1" x14ac:dyDescent="0.3">
@@ -4494,7 +4606,7 @@
         <v>1</v>
       </c>
       <c r="C97" s="11" t="s">
-        <v>406</v>
+        <v>405</v>
       </c>
     </row>
     <row r="98" spans="1:3" s="11" customFormat="1" x14ac:dyDescent="0.3">
@@ -4502,7 +4614,7 @@
         <v>2</v>
       </c>
       <c r="C98" s="11" t="s">
-        <v>407</v>
+        <v>406</v>
       </c>
     </row>
     <row r="99" spans="1:3" s="11" customFormat="1" x14ac:dyDescent="0.3">
@@ -4510,28 +4622,28 @@
         <v>3</v>
       </c>
       <c r="C99" s="11" t="s">
-        <v>409</v>
+        <v>408</v>
       </c>
     </row>
     <row r="100" spans="1:3" s="11" customFormat="1" x14ac:dyDescent="0.3">
       <c r="C100" s="11" t="s">
-        <v>408</v>
+        <v>407</v>
       </c>
     </row>
     <row r="101" spans="1:3" s="11" customFormat="1" x14ac:dyDescent="0.3">
       <c r="C101" s="11" t="s">
-        <v>410</v>
+        <v>409</v>
       </c>
     </row>
     <row r="102" spans="1:3" s="11" customFormat="1" x14ac:dyDescent="0.3"/>
     <row r="103" spans="1:3" s="11" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A103" s="11" t="s">
-        <v>397</v>
+        <v>396</v>
       </c>
     </row>
     <row r="104" spans="1:3" s="11" customFormat="1" x14ac:dyDescent="0.3">
       <c r="B104" s="11" t="s">
-        <v>298</v>
+        <v>297</v>
       </c>
     </row>
     <row r="105" spans="1:3" s="11" customFormat="1" x14ac:dyDescent="0.3">
@@ -4539,23 +4651,23 @@
         <v>1</v>
       </c>
       <c r="C105" s="11" t="s">
-        <v>398</v>
+        <v>397</v>
       </c>
     </row>
     <row r="106" spans="1:3" s="11" customFormat="1" x14ac:dyDescent="0.3">
       <c r="C106" s="11" t="s">
-        <v>399</v>
+        <v>398</v>
       </c>
     </row>
     <row r="107" spans="1:3" s="11" customFormat="1" x14ac:dyDescent="0.3"/>
     <row r="108" spans="1:3" s="11" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A108" s="11" t="s">
-        <v>390</v>
+        <v>389</v>
       </c>
     </row>
     <row r="109" spans="1:3" s="11" customFormat="1" x14ac:dyDescent="0.3">
       <c r="B109" s="11" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
     </row>
     <row r="110" spans="1:3" s="11" customFormat="1" x14ac:dyDescent="0.3">
@@ -4563,12 +4675,12 @@
         <v>1</v>
       </c>
       <c r="C110" s="11" t="s">
-        <v>391</v>
+        <v>390</v>
       </c>
     </row>
     <row r="111" spans="1:3" s="11" customFormat="1" x14ac:dyDescent="0.3">
       <c r="B111" s="11" t="s">
-        <v>298</v>
+        <v>297</v>
       </c>
     </row>
     <row r="112" spans="1:3" s="11" customFormat="1" x14ac:dyDescent="0.3">
@@ -4576,17 +4688,17 @@
         <v>1</v>
       </c>
       <c r="C112" s="11" t="s">
-        <v>392</v>
+        <v>391</v>
       </c>
     </row>
     <row r="113" spans="1:3" s="11" customFormat="1" x14ac:dyDescent="0.3">
       <c r="C113" s="11" t="s">
-        <v>394</v>
+        <v>393</v>
       </c>
     </row>
     <row r="114" spans="1:3" s="11" customFormat="1" x14ac:dyDescent="0.3">
       <c r="B114" s="11" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
     </row>
     <row r="115" spans="1:3" s="11" customFormat="1" x14ac:dyDescent="0.3">
@@ -4594,28 +4706,28 @@
         <v>1</v>
       </c>
       <c r="C115" s="11" t="s">
-        <v>395</v>
+        <v>394</v>
       </c>
     </row>
     <row r="116" spans="1:3" s="11" customFormat="1" x14ac:dyDescent="0.3">
       <c r="C116" s="11" t="s">
-        <v>393</v>
+        <v>392</v>
       </c>
     </row>
     <row r="117" spans="1:3" s="11" customFormat="1" x14ac:dyDescent="0.3">
       <c r="C117" s="11" t="s">
-        <v>396</v>
+        <v>395</v>
       </c>
     </row>
     <row r="118" spans="1:3" s="11" customFormat="1" x14ac:dyDescent="0.3"/>
     <row r="119" spans="1:3" s="11" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A119" s="11" t="s">
-        <v>384</v>
+        <v>383</v>
       </c>
     </row>
     <row r="120" spans="1:3" s="11" customFormat="1" x14ac:dyDescent="0.3">
       <c r="B120" s="11" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
     </row>
     <row r="121" spans="1:3" s="11" customFormat="1" x14ac:dyDescent="0.3">
@@ -4623,7 +4735,7 @@
         <v>1</v>
       </c>
       <c r="C121" s="11" t="s">
-        <v>385</v>
+        <v>384</v>
       </c>
     </row>
     <row r="122" spans="1:3" s="11" customFormat="1" x14ac:dyDescent="0.3">
@@ -4631,12 +4743,12 @@
         <v>2</v>
       </c>
       <c r="C122" s="11" t="s">
-        <v>386</v>
+        <v>385</v>
       </c>
     </row>
     <row r="123" spans="1:3" s="11" customFormat="1" x14ac:dyDescent="0.3">
       <c r="B123" s="11" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
     </row>
     <row r="124" spans="1:3" s="11" customFormat="1" x14ac:dyDescent="0.3">
@@ -4644,7 +4756,7 @@
         <v>1</v>
       </c>
       <c r="C124" s="11" t="s">
-        <v>387</v>
+        <v>386</v>
       </c>
     </row>
     <row r="125" spans="1:3" s="11" customFormat="1" x14ac:dyDescent="0.3">
@@ -4652,7 +4764,7 @@
         <v>2</v>
       </c>
       <c r="C125" s="11" t="s">
-        <v>388</v>
+        <v>387</v>
       </c>
     </row>
     <row r="126" spans="1:3" s="11" customFormat="1" x14ac:dyDescent="0.3">
@@ -4660,18 +4772,18 @@
         <v>3</v>
       </c>
       <c r="C126" s="11" t="s">
-        <v>389</v>
+        <v>388</v>
       </c>
     </row>
     <row r="127" spans="1:3" s="11" customFormat="1" x14ac:dyDescent="0.3"/>
     <row r="128" spans="1:3" s="11" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A128" s="11" t="s">
-        <v>369</v>
+        <v>368</v>
       </c>
     </row>
     <row r="129" spans="2:30" s="11" customFormat="1" x14ac:dyDescent="0.3">
       <c r="B129" s="11" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
     </row>
     <row r="130" spans="2:30" s="11" customFormat="1" x14ac:dyDescent="0.3">
@@ -4679,12 +4791,12 @@
         <v>1</v>
       </c>
       <c r="C130" s="11" t="s">
-        <v>370</v>
+        <v>369</v>
       </c>
     </row>
     <row r="131" spans="2:30" s="11" customFormat="1" x14ac:dyDescent="0.3">
       <c r="B131" s="11" t="s">
-        <v>298</v>
+        <v>297</v>
       </c>
     </row>
     <row r="132" spans="2:30" s="11" customFormat="1" x14ac:dyDescent="0.3">
@@ -4692,12 +4804,12 @@
         <v>1</v>
       </c>
       <c r="C132" s="11" t="s">
-        <v>373</v>
+        <v>372</v>
       </c>
     </row>
     <row r="133" spans="2:30" s="11" customFormat="1" x14ac:dyDescent="0.3">
       <c r="B133" s="11" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
     </row>
     <row r="134" spans="2:30" s="11" customFormat="1" x14ac:dyDescent="0.3">
@@ -4705,7 +4817,7 @@
         <v>1</v>
       </c>
       <c r="C134" s="11" t="s">
-        <v>377</v>
+        <v>376</v>
       </c>
     </row>
     <row r="135" spans="2:30" s="11" customFormat="1" x14ac:dyDescent="0.3">
@@ -4713,33 +4825,33 @@
         <v>2</v>
       </c>
       <c r="C135" s="11" t="s">
-        <v>371</v>
+        <v>370</v>
       </c>
     </row>
     <row r="136" spans="2:30" s="11" customFormat="1" x14ac:dyDescent="0.3">
       <c r="C136" s="11" t="s">
-        <v>379</v>
+        <v>378</v>
       </c>
     </row>
     <row r="137" spans="2:30" s="11" customFormat="1" x14ac:dyDescent="0.3">
       <c r="C137" s="11" t="s">
-        <v>380</v>
+        <v>379</v>
       </c>
       <c r="AD137" s="15"/>
     </row>
     <row r="138" spans="2:30" s="11" customFormat="1" x14ac:dyDescent="0.3">
       <c r="D138" s="11" t="s">
-        <v>382</v>
+        <v>381</v>
       </c>
     </row>
     <row r="139" spans="2:30" s="11" customFormat="1" x14ac:dyDescent="0.3">
       <c r="D139" s="11" t="s">
-        <v>381</v>
+        <v>380</v>
       </c>
     </row>
     <row r="140" spans="2:30" s="11" customFormat="1" x14ac:dyDescent="0.3">
       <c r="D140" s="14" t="s">
-        <v>383</v>
+        <v>382</v>
       </c>
     </row>
     <row r="141" spans="2:30" s="11" customFormat="1" x14ac:dyDescent="0.3">
@@ -4747,7 +4859,7 @@
         <v>3</v>
       </c>
       <c r="C141" s="11" t="s">
-        <v>372</v>
+        <v>371</v>
       </c>
     </row>
     <row r="142" spans="2:30" s="11" customFormat="1" x14ac:dyDescent="0.3">
@@ -4755,7 +4867,7 @@
         <v>4</v>
       </c>
       <c r="C142" s="11" t="s">
-        <v>374</v>
+        <v>373</v>
       </c>
     </row>
     <row r="143" spans="2:30" s="11" customFormat="1" x14ac:dyDescent="0.3">
@@ -4763,12 +4875,12 @@
         <v>5</v>
       </c>
       <c r="C143" s="11" t="s">
-        <v>375</v>
+        <v>374</v>
       </c>
     </row>
     <row r="144" spans="2:30" s="11" customFormat="1" x14ac:dyDescent="0.3">
       <c r="C144" s="11" t="s">
-        <v>376</v>
+        <v>375</v>
       </c>
     </row>
     <row r="145" spans="1:3" s="11" customFormat="1" x14ac:dyDescent="0.3">
@@ -4776,18 +4888,18 @@
         <v>6</v>
       </c>
       <c r="C145" s="11" t="s">
-        <v>378</v>
+        <v>377</v>
       </c>
     </row>
     <row r="146" spans="1:3" s="11" customFormat="1" x14ac:dyDescent="0.3"/>
     <row r="147" spans="1:3" s="11" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A147" s="11" t="s">
-        <v>324</v>
+        <v>323</v>
       </c>
     </row>
     <row r="148" spans="1:3" s="11" customFormat="1" x14ac:dyDescent="0.3">
       <c r="B148" s="11" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
     </row>
     <row r="149" spans="1:3" s="11" customFormat="1" x14ac:dyDescent="0.3">
@@ -4795,7 +4907,7 @@
         <v>1</v>
       </c>
       <c r="C149" s="11" t="s">
-        <v>325</v>
+        <v>324</v>
       </c>
     </row>
     <row r="150" spans="1:3" s="11" customFormat="1" x14ac:dyDescent="0.3">
@@ -4803,18 +4915,18 @@
         <v>2</v>
       </c>
       <c r="C150" s="11" t="s">
-        <v>326</v>
+        <v>325</v>
       </c>
     </row>
     <row r="151" spans="1:3" s="11" customFormat="1" x14ac:dyDescent="0.3"/>
     <row r="152" spans="1:3" s="11" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A152" s="11" t="s">
-        <v>320</v>
+        <v>319</v>
       </c>
     </row>
     <row r="153" spans="1:3" s="11" customFormat="1" x14ac:dyDescent="0.3">
       <c r="B153" s="11" t="s">
-        <v>298</v>
+        <v>297</v>
       </c>
     </row>
     <row r="154" spans="1:3" s="11" customFormat="1" x14ac:dyDescent="0.3">
@@ -4822,12 +4934,12 @@
         <v>1</v>
       </c>
       <c r="C154" s="11" t="s">
-        <v>321</v>
+        <v>320</v>
       </c>
     </row>
     <row r="155" spans="1:3" s="11" customFormat="1" x14ac:dyDescent="0.3">
       <c r="B155" s="11" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
     </row>
     <row r="156" spans="1:3" s="11" customFormat="1" x14ac:dyDescent="0.3">
@@ -4835,23 +4947,23 @@
         <v>1</v>
       </c>
       <c r="C156" s="11" t="s">
-        <v>322</v>
+        <v>321</v>
       </c>
     </row>
     <row r="157" spans="1:3" s="11" customFormat="1" x14ac:dyDescent="0.3">
       <c r="C157" s="11" t="s">
-        <v>323</v>
+        <v>322</v>
       </c>
     </row>
     <row r="158" spans="1:3" s="11" customFormat="1" x14ac:dyDescent="0.3"/>
     <row r="159" spans="1:3" s="11" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A159" s="11" t="s">
-        <v>297</v>
+        <v>296</v>
       </c>
     </row>
     <row r="160" spans="1:3" s="11" customFormat="1" x14ac:dyDescent="0.3">
       <c r="B160" s="11" t="s">
-        <v>298</v>
+        <v>297</v>
       </c>
     </row>
     <row r="161" spans="1:4" s="11" customFormat="1" x14ac:dyDescent="0.3">
@@ -4859,7 +4971,7 @@
         <v>1</v>
       </c>
       <c r="C161" s="11" t="s">
-        <v>308</v>
+        <v>307</v>
       </c>
     </row>
     <row r="162" spans="1:4" s="11" customFormat="1" x14ac:dyDescent="0.3">
@@ -4867,12 +4979,12 @@
         <v>2</v>
       </c>
       <c r="C162" s="11" t="s">
-        <v>300</v>
+        <v>299</v>
       </c>
     </row>
     <row r="163" spans="1:4" s="11" customFormat="1" x14ac:dyDescent="0.3">
       <c r="B163" s="11" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
     </row>
     <row r="164" spans="1:4" s="11" customFormat="1" x14ac:dyDescent="0.3">
@@ -4880,7 +4992,7 @@
         <v>1</v>
       </c>
       <c r="C164" s="11" t="s">
-        <v>301</v>
+        <v>300</v>
       </c>
     </row>
     <row r="165" spans="1:4" s="11" customFormat="1" x14ac:dyDescent="0.3">
@@ -4888,7 +5000,7 @@
         <v>2</v>
       </c>
       <c r="C165" s="11" t="s">
-        <v>299</v>
+        <v>298</v>
       </c>
     </row>
     <row r="166" spans="1:4" s="11" customFormat="1" x14ac:dyDescent="0.3">
@@ -4896,37 +5008,37 @@
         <v>3</v>
       </c>
       <c r="C166" s="11" t="s">
-        <v>302</v>
+        <v>301</v>
       </c>
     </row>
     <row r="167" spans="1:4" s="11" customFormat="1" x14ac:dyDescent="0.3">
       <c r="C167" s="11" t="s">
-        <v>309</v>
+        <v>308</v>
       </c>
     </row>
     <row r="168" spans="1:4" s="11" customFormat="1" x14ac:dyDescent="0.3">
       <c r="C168" s="11" t="s">
-        <v>306</v>
+        <v>305</v>
       </c>
     </row>
     <row r="169" spans="1:4" s="11" customFormat="1" x14ac:dyDescent="0.3">
       <c r="D169" s="11" t="s">
-        <v>303</v>
+        <v>302</v>
       </c>
     </row>
     <row r="170" spans="1:4" s="11" customFormat="1" x14ac:dyDescent="0.3">
       <c r="D170" s="11" t="s">
-        <v>304</v>
+        <v>303</v>
       </c>
     </row>
     <row r="171" spans="1:4" s="11" customFormat="1" x14ac:dyDescent="0.3">
       <c r="D171" s="11" t="s">
-        <v>305</v>
+        <v>304</v>
       </c>
     </row>
     <row r="172" spans="1:4" s="11" customFormat="1" x14ac:dyDescent="0.3">
       <c r="C172" s="11" t="s">
-        <v>310</v>
+        <v>309</v>
       </c>
     </row>
     <row r="173" spans="1:4" s="11" customFormat="1" x14ac:dyDescent="0.3">
@@ -4934,18 +5046,18 @@
         <v>4</v>
       </c>
       <c r="C173" s="11" t="s">
-        <v>307</v>
+        <v>306</v>
       </c>
     </row>
     <row r="174" spans="1:4" s="11" customFormat="1" x14ac:dyDescent="0.3"/>
     <row r="175" spans="1:4" s="11" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A175" s="11" t="s">
-        <v>295</v>
+        <v>294</v>
       </c>
     </row>
     <row r="176" spans="1:4" s="11" customFormat="1" x14ac:dyDescent="0.3">
       <c r="B176" s="11" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
     </row>
     <row r="177" spans="1:3" s="11" customFormat="1" x14ac:dyDescent="0.3">
@@ -4953,12 +5065,12 @@
         <v>1</v>
       </c>
       <c r="C177" s="11" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
     </row>
     <row r="178" spans="1:3" s="11" customFormat="1" x14ac:dyDescent="0.3">
       <c r="B178" s="11" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
     </row>
     <row r="179" spans="1:3" s="11" customFormat="1" x14ac:dyDescent="0.3">
@@ -4966,7 +5078,7 @@
         <v>1</v>
       </c>
       <c r="C179" s="11" t="s">
-        <v>293</v>
+        <v>292</v>
       </c>
     </row>
     <row r="180" spans="1:3" s="11" customFormat="1" x14ac:dyDescent="0.3">
@@ -4974,7 +5086,7 @@
         <v>2</v>
       </c>
       <c r="C180" s="11" t="s">
-        <v>292</v>
+        <v>291</v>
       </c>
     </row>
     <row r="181" spans="1:3" s="11" customFormat="1" x14ac:dyDescent="0.3">
@@ -4982,18 +5094,18 @@
         <v>3</v>
       </c>
       <c r="C181" s="11" t="s">
-        <v>294</v>
+        <v>293</v>
       </c>
     </row>
     <row r="182" spans="1:3" s="11" customFormat="1" x14ac:dyDescent="0.3"/>
     <row r="183" spans="1:3" s="11" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A183" s="11" t="s">
-        <v>289</v>
+        <v>288</v>
       </c>
     </row>
     <row r="184" spans="1:3" s="11" customFormat="1" x14ac:dyDescent="0.3">
       <c r="B184" s="11" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
     </row>
     <row r="185" spans="1:3" s="11" customFormat="1" x14ac:dyDescent="0.3">
@@ -5001,23 +5113,23 @@
         <v>1</v>
       </c>
       <c r="C185" s="11" t="s">
-        <v>290</v>
+        <v>289</v>
       </c>
     </row>
     <row r="186" spans="1:3" s="11" customFormat="1" x14ac:dyDescent="0.3">
       <c r="C186" s="11" t="s">
-        <v>291</v>
+        <v>290</v>
       </c>
     </row>
     <row r="187" spans="1:3" s="11" customFormat="1" x14ac:dyDescent="0.3"/>
     <row r="188" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A188" t="s">
-        <v>276</v>
+        <v>275</v>
       </c>
     </row>
     <row r="189" spans="1:3" x14ac:dyDescent="0.3">
       <c r="B189" t="s">
-        <v>287</v>
+        <v>286</v>
       </c>
     </row>
     <row r="190" spans="1:3" x14ac:dyDescent="0.3">
@@ -5025,12 +5137,12 @@
         <v>1</v>
       </c>
       <c r="C190" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
     </row>
     <row r="191" spans="1:3" x14ac:dyDescent="0.3">
       <c r="B191" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
     </row>
     <row r="192" spans="1:3" x14ac:dyDescent="0.3">
@@ -5038,7 +5150,7 @@
         <v>1</v>
       </c>
       <c r="C192" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
     </row>
     <row r="193" spans="1:3" x14ac:dyDescent="0.3">
@@ -5046,17 +5158,17 @@
         <v>2</v>
       </c>
       <c r="C193" t="s">
-        <v>277</v>
+        <v>276</v>
       </c>
     </row>
     <row r="194" spans="1:3" x14ac:dyDescent="0.3">
       <c r="C194" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
     </row>
     <row r="195" spans="1:3" x14ac:dyDescent="0.3">
       <c r="B195" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
     </row>
     <row r="196" spans="1:3" x14ac:dyDescent="0.3">
@@ -5064,12 +5176,12 @@
         <v>1</v>
       </c>
       <c r="C196" t="s">
-        <v>286</v>
+        <v>285</v>
       </c>
     </row>
     <row r="197" spans="1:3" x14ac:dyDescent="0.3">
       <c r="B197" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
     </row>
     <row r="198" spans="1:3" x14ac:dyDescent="0.3">
@@ -5077,7 +5189,7 @@
         <v>1</v>
       </c>
       <c r="C198" t="s">
-        <v>282</v>
+        <v>281</v>
       </c>
     </row>
     <row r="199" spans="1:3" x14ac:dyDescent="0.3">
@@ -5085,7 +5197,7 @@
         <v>2</v>
       </c>
       <c r="C199" t="s">
-        <v>283</v>
+        <v>282</v>
       </c>
     </row>
     <row r="200" spans="1:3" x14ac:dyDescent="0.3">
@@ -5093,7 +5205,7 @@
         <v>3</v>
       </c>
       <c r="C200" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
     </row>
     <row r="201" spans="1:3" x14ac:dyDescent="0.3">
@@ -5101,7 +5213,7 @@
         <v>4</v>
       </c>
       <c r="C201" t="s">
-        <v>281</v>
+        <v>280</v>
       </c>
     </row>
     <row r="202" spans="1:3" x14ac:dyDescent="0.3">
@@ -5109,22 +5221,22 @@
         <v>5</v>
       </c>
       <c r="C202" t="s">
-        <v>284</v>
+        <v>283</v>
       </c>
     </row>
     <row r="203" spans="1:3" x14ac:dyDescent="0.3">
       <c r="C203" t="s">
-        <v>285</v>
+        <v>284</v>
       </c>
     </row>
     <row r="205" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A205" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
     </row>
     <row r="206" spans="1:3" x14ac:dyDescent="0.3">
       <c r="B206" t="s">
-        <v>275</v>
+        <v>274</v>
       </c>
     </row>
     <row r="207" spans="1:3" x14ac:dyDescent="0.3">
@@ -5132,7 +5244,7 @@
         <v>1</v>
       </c>
       <c r="C207" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
     </row>
     <row r="208" spans="1:3" x14ac:dyDescent="0.3">
@@ -5140,7 +5252,7 @@
         <v>2</v>
       </c>
       <c r="C208" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
     </row>
     <row r="209" spans="1:3" x14ac:dyDescent="0.3">
@@ -5148,7 +5260,7 @@
         <v>3</v>
       </c>
       <c r="C209" t="s">
-        <v>268</v>
+        <v>267</v>
       </c>
     </row>
     <row r="210" spans="1:3" x14ac:dyDescent="0.3">
@@ -5156,7 +5268,7 @@
         <v>4</v>
       </c>
       <c r="C210" t="s">
-        <v>269</v>
+        <v>268</v>
       </c>
     </row>
     <row r="211" spans="1:3" x14ac:dyDescent="0.3">
@@ -5164,7 +5276,7 @@
         <v>5</v>
       </c>
       <c r="C211" t="s">
-        <v>270</v>
+        <v>269</v>
       </c>
     </row>
     <row r="212" spans="1:3" x14ac:dyDescent="0.3">
@@ -5172,7 +5284,7 @@
         <v>6</v>
       </c>
       <c r="C212" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
     </row>
     <row r="213" spans="1:3" x14ac:dyDescent="0.3">
@@ -5180,7 +5292,7 @@
         <v>7</v>
       </c>
       <c r="C213" t="s">
-        <v>272</v>
+        <v>271</v>
       </c>
     </row>
     <row r="214" spans="1:3" x14ac:dyDescent="0.3">
@@ -5188,7 +5300,7 @@
         <v>8</v>
       </c>
       <c r="C214" t="s">
-        <v>273</v>
+        <v>272</v>
       </c>
     </row>
     <row r="215" spans="1:3" x14ac:dyDescent="0.3">
@@ -5196,17 +5308,17 @@
         <v>9</v>
       </c>
       <c r="C215" t="s">
-        <v>274</v>
+        <v>273</v>
       </c>
     </row>
     <row r="217" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A217" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
     </row>
     <row r="218" spans="1:3" x14ac:dyDescent="0.3">
       <c r="B218" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
     </row>
     <row r="219" spans="1:3" x14ac:dyDescent="0.3">
@@ -5214,17 +5326,17 @@
         <v>1</v>
       </c>
       <c r="C219" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
     </row>
     <row r="221" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A221" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
     </row>
     <row r="222" spans="1:3" x14ac:dyDescent="0.3">
       <c r="B222" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
     </row>
     <row r="223" spans="1:3" x14ac:dyDescent="0.3">
@@ -5232,17 +5344,17 @@
         <v>1</v>
       </c>
       <c r="C223" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
     </row>
     <row r="225" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A225" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
     </row>
     <row r="226" spans="1:3" x14ac:dyDescent="0.3">
       <c r="B226" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
     </row>
     <row r="227" spans="1:3" x14ac:dyDescent="0.3">
@@ -5250,7 +5362,7 @@
         <v>1</v>
       </c>
       <c r="C227" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
     </row>
     <row r="228" spans="1:3" x14ac:dyDescent="0.3">
@@ -5258,12 +5370,12 @@
         <v>2</v>
       </c>
       <c r="C228" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
     </row>
     <row r="229" spans="1:3" x14ac:dyDescent="0.3">
       <c r="B229" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
     </row>
     <row r="230" spans="1:3" x14ac:dyDescent="0.3">
@@ -5271,27 +5383,27 @@
         <v>1</v>
       </c>
       <c r="C230" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
     </row>
     <row r="232" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A232" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
     </row>
     <row r="233" spans="1:3" x14ac:dyDescent="0.3">
       <c r="B233" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
     </row>
     <row r="234" spans="1:3" x14ac:dyDescent="0.3">
       <c r="C234" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
     </row>
     <row r="235" spans="1:3" x14ac:dyDescent="0.3">
       <c r="B235" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
     </row>
     <row r="236" spans="1:3" x14ac:dyDescent="0.3">
@@ -5299,7 +5411,7 @@
         <v>1</v>
       </c>
       <c r="C236" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
     </row>
     <row r="237" spans="1:3" x14ac:dyDescent="0.3">
@@ -5307,7 +5419,7 @@
         <v>2</v>
       </c>
       <c r="C237" t="s">
-        <v>251</v>
+        <v>250</v>
       </c>
     </row>
     <row r="238" spans="1:3" x14ac:dyDescent="0.3">
@@ -5315,12 +5427,12 @@
         <v>3</v>
       </c>
       <c r="C238" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
     </row>
     <row r="240" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A240" s="11" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="B240" s="11"/>
       <c r="C240" s="11"/>
@@ -5328,7 +5440,7 @@
     <row r="241" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A241" s="11"/>
       <c r="B241" s="11" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="C241" s="11"/>
     </row>
@@ -5338,7 +5450,7 @@
         <v>1</v>
       </c>
       <c r="C242" s="11" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
     </row>
     <row r="243" spans="1:4" x14ac:dyDescent="0.3">
@@ -5347,13 +5459,13 @@
         <v>2</v>
       </c>
       <c r="C243" s="11" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
     </row>
     <row r="244" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A244" s="11"/>
       <c r="B244" s="11" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="C244" s="11"/>
     </row>
@@ -5363,7 +5475,7 @@
         <v>1</v>
       </c>
       <c r="C245" s="11" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
     </row>
     <row r="246" spans="1:4" x14ac:dyDescent="0.3">
@@ -5372,21 +5484,21 @@
         <v>2</v>
       </c>
       <c r="C246" s="11" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
     </row>
     <row r="247" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A247" s="11"/>
       <c r="B247" s="11"/>
       <c r="C247" s="11" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
     </row>
     <row r="248" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A248" s="11"/>
       <c r="B248" s="11"/>
       <c r="C248" s="11" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
       <c r="D248" s="11"/>
     </row>
@@ -5394,7 +5506,7 @@
       <c r="A249" s="11"/>
       <c r="B249" s="11"/>
       <c r="C249" s="11" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="D249" s="11"/>
     </row>
@@ -5403,14 +5515,14 @@
       <c r="B250" s="11"/>
       <c r="C250" s="11"/>
       <c r="D250" s="11" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
     </row>
     <row r="251" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A251" s="11"/>
       <c r="B251" s="11"/>
       <c r="C251" s="11" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
       <c r="D251" s="11"/>
     </row>
@@ -5419,21 +5531,21 @@
       <c r="B252" s="11"/>
       <c r="C252" s="11"/>
       <c r="D252" s="11" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
     </row>
     <row r="253" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A253" s="11"/>
       <c r="B253" s="11"/>
       <c r="C253" s="11" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
       <c r="D253" s="11"/>
     </row>
     <row r="254" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A254" s="11"/>
       <c r="B254" s="11" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="C254" s="11"/>
       <c r="D254" s="11"/>
@@ -5444,14 +5556,14 @@
         <v>1</v>
       </c>
       <c r="C255" s="11" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
       <c r="D255" s="11"/>
     </row>
     <row r="256" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A256" s="11"/>
       <c r="B256" s="11" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="C256" s="11"/>
       <c r="D256" s="11"/>
@@ -5462,14 +5574,14 @@
         <v>1</v>
       </c>
       <c r="C257" s="11" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
       <c r="D257" s="11"/>
     </row>
     <row r="258" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A258" s="11"/>
       <c r="B258" s="11" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
       <c r="C258" s="11"/>
       <c r="D258" s="11"/>
@@ -5480,18 +5592,18 @@
         <v>1</v>
       </c>
       <c r="C259" s="11" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
       <c r="D259" s="11"/>
     </row>
     <row r="261" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A261" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
     </row>
     <row r="262" spans="1:4" x14ac:dyDescent="0.3">
       <c r="B262" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
     </row>
     <row r="263" spans="1:4" x14ac:dyDescent="0.3">
@@ -5499,7 +5611,7 @@
         <v>1</v>
       </c>
       <c r="C263" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
     </row>
     <row r="264" spans="1:4" x14ac:dyDescent="0.3">
@@ -5507,7 +5619,7 @@
         <v>2</v>
       </c>
       <c r="C264" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
     </row>
     <row r="265" spans="1:4" x14ac:dyDescent="0.3">
@@ -5515,7 +5627,7 @@
         <v>3</v>
       </c>
       <c r="C265" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
     </row>
     <row r="266" spans="1:4" x14ac:dyDescent="0.3">
@@ -5523,12 +5635,12 @@
         <v>4</v>
       </c>
       <c r="C266" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
     </row>
     <row r="267" spans="1:4" x14ac:dyDescent="0.3">
       <c r="B267" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
     </row>
     <row r="268" spans="1:4" x14ac:dyDescent="0.3">
@@ -5536,17 +5648,17 @@
         <v>1</v>
       </c>
       <c r="C268" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
     </row>
     <row r="269" spans="1:4" x14ac:dyDescent="0.3">
       <c r="C269" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
     </row>
     <row r="270" spans="1:4" x14ac:dyDescent="0.3">
       <c r="C270" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
     </row>
     <row r="271" spans="1:4" x14ac:dyDescent="0.3">
@@ -5554,12 +5666,12 @@
         <v>2</v>
       </c>
       <c r="C271" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
     </row>
     <row r="272" spans="1:4" x14ac:dyDescent="0.3">
       <c r="B272" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
     </row>
     <row r="273" spans="1:3" x14ac:dyDescent="0.3">
@@ -5567,22 +5679,22 @@
         <v>1</v>
       </c>
       <c r="C273" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
     </row>
     <row r="274" spans="1:3" x14ac:dyDescent="0.3">
       <c r="C274" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
     </row>
     <row r="275" spans="1:3" x14ac:dyDescent="0.3">
       <c r="C275" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
     </row>
     <row r="276" spans="1:3" x14ac:dyDescent="0.3">
       <c r="C276" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
     </row>
     <row r="277" spans="1:3" x14ac:dyDescent="0.3">
@@ -5590,12 +5702,12 @@
         <v>2</v>
       </c>
       <c r="C277" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
     </row>
     <row r="278" spans="1:3" x14ac:dyDescent="0.3">
       <c r="B278" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
     </row>
     <row r="279" spans="1:3" x14ac:dyDescent="0.3">
@@ -5603,17 +5715,17 @@
         <v>1</v>
       </c>
       <c r="C279" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
     </row>
     <row r="281" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A281" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
     </row>
     <row r="282" spans="1:3" x14ac:dyDescent="0.3">
       <c r="B282" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
     </row>
     <row r="283" spans="1:3" x14ac:dyDescent="0.3">
@@ -5621,7 +5733,7 @@
         <v>1</v>
       </c>
       <c r="C283" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
     </row>
     <row r="284" spans="1:3" x14ac:dyDescent="0.3">
@@ -5629,7 +5741,7 @@
         <v>2</v>
       </c>
       <c r="C284" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
     </row>
     <row r="285" spans="1:3" x14ac:dyDescent="0.3">
@@ -5637,7 +5749,7 @@
         <v>3</v>
       </c>
       <c r="C285" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
     </row>
     <row r="286" spans="1:3" x14ac:dyDescent="0.3">
@@ -5645,12 +5757,12 @@
         <v>4</v>
       </c>
       <c r="C286" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
     </row>
     <row r="287" spans="1:3" x14ac:dyDescent="0.3">
       <c r="B287" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
     </row>
     <row r="288" spans="1:3" x14ac:dyDescent="0.3">
@@ -5658,22 +5770,22 @@
         <v>1</v>
       </c>
       <c r="C288" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
     </row>
     <row r="289" spans="1:4" x14ac:dyDescent="0.3">
       <c r="C289" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
     </row>
     <row r="290" spans="1:4" x14ac:dyDescent="0.3">
       <c r="C290" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
     </row>
     <row r="291" spans="1:4" x14ac:dyDescent="0.3">
       <c r="B291" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
     </row>
     <row r="292" spans="1:4" x14ac:dyDescent="0.3">
@@ -5681,7 +5793,7 @@
         <v>1</v>
       </c>
       <c r="C292" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
     </row>
     <row r="293" spans="1:4" x14ac:dyDescent="0.3">
@@ -5689,22 +5801,22 @@
         <v>2</v>
       </c>
       <c r="C293" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
     </row>
     <row r="294" spans="1:4" x14ac:dyDescent="0.3">
       <c r="C294" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
     </row>
     <row r="295" spans="1:4" x14ac:dyDescent="0.3">
       <c r="C295" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
     </row>
     <row r="296" spans="1:4" x14ac:dyDescent="0.3">
       <c r="B296" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
     </row>
     <row r="297" spans="1:4" x14ac:dyDescent="0.3">
@@ -5712,17 +5824,17 @@
         <v>1</v>
       </c>
       <c r="C297" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
     </row>
     <row r="299" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A299" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
     </row>
     <row r="300" spans="1:4" x14ac:dyDescent="0.3">
       <c r="B300" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
     </row>
     <row r="301" spans="1:4" x14ac:dyDescent="0.3">
@@ -5730,7 +5842,7 @@
         <v>1</v>
       </c>
       <c r="C301" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
     </row>
     <row r="302" spans="1:4" x14ac:dyDescent="0.3">
@@ -5738,7 +5850,7 @@
         <v>2</v>
       </c>
       <c r="C302" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
     </row>
     <row r="303" spans="1:4" x14ac:dyDescent="0.3">
@@ -5746,15 +5858,15 @@
         <v>3</v>
       </c>
       <c r="C303" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
     </row>
     <row r="304" spans="1:4" x14ac:dyDescent="0.3">
       <c r="B304" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="D304" s="10" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
     </row>
     <row r="305" spans="1:4" x14ac:dyDescent="0.3">
@@ -5762,28 +5874,28 @@
         <v>1</v>
       </c>
       <c r="C305" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
     </row>
     <row r="306" spans="1:4" x14ac:dyDescent="0.3">
       <c r="D306" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
     </row>
     <row r="307" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A307" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="D307" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
     </row>
     <row r="308" spans="1:4" x14ac:dyDescent="0.3">
       <c r="B308" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="D308" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
     </row>
     <row r="309" spans="1:4" x14ac:dyDescent="0.3">
@@ -5791,12 +5903,12 @@
         <v>1</v>
       </c>
       <c r="C309" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
     </row>
     <row r="310" spans="1:4" x14ac:dyDescent="0.3">
       <c r="B310" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
     </row>
     <row r="311" spans="1:4" x14ac:dyDescent="0.3">
@@ -5804,17 +5916,17 @@
         <v>1</v>
       </c>
       <c r="C311" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
     </row>
     <row r="312" spans="1:4" x14ac:dyDescent="0.3">
       <c r="C312" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
     </row>
     <row r="313" spans="1:4" x14ac:dyDescent="0.3">
       <c r="C313" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
     </row>
     <row r="315" spans="1:4" x14ac:dyDescent="0.3">
@@ -5822,7 +5934,7 @@
         <v>2</v>
       </c>
       <c r="C315" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
     </row>
     <row r="319" spans="1:4" x14ac:dyDescent="0.3">
@@ -5830,12 +5942,12 @@
         <v>3</v>
       </c>
       <c r="C319" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
     </row>
     <row r="320" spans="1:4" x14ac:dyDescent="0.3">
       <c r="B320" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
     </row>
     <row r="321" spans="1:4" x14ac:dyDescent="0.3">
@@ -5843,15 +5955,15 @@
         <v>1</v>
       </c>
       <c r="C321" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
     </row>
     <row r="322" spans="1:4" x14ac:dyDescent="0.3">
       <c r="C322" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="D322" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
     </row>
     <row r="323" spans="1:4" x14ac:dyDescent="0.3">
@@ -5859,30 +5971,30 @@
         <v>2</v>
       </c>
       <c r="C323" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
     </row>
     <row r="324" spans="1:4" x14ac:dyDescent="0.3">
       <c r="C324" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
     </row>
     <row r="325" spans="1:4" x14ac:dyDescent="0.3">
       <c r="D325" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
     </row>
     <row r="326" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A326" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="D326" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
     </row>
     <row r="327" spans="1:4" x14ac:dyDescent="0.3">
       <c r="B327" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
     </row>
     <row r="328" spans="1:4" x14ac:dyDescent="0.3">
@@ -5890,18 +6002,18 @@
         <v>1</v>
       </c>
       <c r="C328" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="D328" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
     </row>
     <row r="329" spans="1:4" x14ac:dyDescent="0.3">
       <c r="B329" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="D329" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
     </row>
     <row r="330" spans="1:4" x14ac:dyDescent="0.3">
@@ -5909,30 +6021,30 @@
         <v>1</v>
       </c>
       <c r="C330" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="D330" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
     </row>
     <row r="331" spans="1:4" x14ac:dyDescent="0.3">
       <c r="C331" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
     </row>
     <row r="333" spans="1:4" x14ac:dyDescent="0.3">
       <c r="C333" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
     </row>
     <row r="334" spans="1:4" x14ac:dyDescent="0.3">
       <c r="C334" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
     </row>
     <row r="337" spans="1:3" x14ac:dyDescent="0.3">
       <c r="C337" s="9" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
     </row>
     <row r="338" spans="1:3" x14ac:dyDescent="0.3">
@@ -5946,17 +6058,17 @@
     </row>
     <row r="341" spans="1:3" x14ac:dyDescent="0.3">
       <c r="C341" s="9" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
     </row>
     <row r="343" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A343" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
     </row>
     <row r="344" spans="1:3" x14ac:dyDescent="0.3">
       <c r="B344" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
     </row>
     <row r="345" spans="1:3" x14ac:dyDescent="0.3">
@@ -5964,7 +6076,7 @@
         <v>1</v>
       </c>
       <c r="C345" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
     </row>
     <row r="346" spans="1:3" x14ac:dyDescent="0.3">
@@ -5972,17 +6084,17 @@
         <v>2</v>
       </c>
       <c r="C346" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
     </row>
     <row r="348" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A348" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
     </row>
     <row r="349" spans="1:3" x14ac:dyDescent="0.3">
       <c r="B349" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
     </row>
     <row r="350" spans="1:3" x14ac:dyDescent="0.3">
@@ -5990,7 +6102,7 @@
         <v>1</v>
       </c>
       <c r="C350" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
     </row>
     <row r="351" spans="1:3" x14ac:dyDescent="0.3">
@@ -5998,12 +6110,12 @@
         <v>2</v>
       </c>
       <c r="C351" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
     </row>
     <row r="352" spans="1:3" x14ac:dyDescent="0.3">
       <c r="B352" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
     </row>
     <row r="353" spans="1:3" x14ac:dyDescent="0.3">
@@ -6011,12 +6123,12 @@
         <v>1</v>
       </c>
       <c r="C353" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
     </row>
     <row r="354" spans="1:3" x14ac:dyDescent="0.3">
       <c r="B354" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
     </row>
     <row r="355" spans="1:3" x14ac:dyDescent="0.3">
@@ -6024,17 +6136,17 @@
         <v>1</v>
       </c>
       <c r="C355" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
     </row>
     <row r="357" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A357" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
     </row>
     <row r="358" spans="1:3" x14ac:dyDescent="0.3">
       <c r="B358" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
     </row>
     <row r="359" spans="1:3" x14ac:dyDescent="0.3">
@@ -6042,7 +6154,7 @@
         <v>1</v>
       </c>
       <c r="C359" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
     </row>
     <row r="360" spans="1:3" x14ac:dyDescent="0.3">
@@ -6050,7 +6162,7 @@
         <v>2</v>
       </c>
       <c r="C360" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
     </row>
     <row r="361" spans="1:3" x14ac:dyDescent="0.3">
@@ -6058,12 +6170,12 @@
         <v>3</v>
       </c>
       <c r="C361" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
     </row>
     <row r="362" spans="1:3" x14ac:dyDescent="0.3">
       <c r="B362" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
     </row>
     <row r="363" spans="1:3" x14ac:dyDescent="0.3">
@@ -6071,7 +6183,7 @@
         <v>1</v>
       </c>
       <c r="C363" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
     </row>
     <row r="364" spans="1:3" x14ac:dyDescent="0.3">
@@ -6079,12 +6191,12 @@
         <v>2</v>
       </c>
       <c r="C364" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
     </row>
     <row r="365" spans="1:3" x14ac:dyDescent="0.3">
       <c r="C365" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
     </row>
     <row r="366" spans="1:3" x14ac:dyDescent="0.3">
@@ -6092,17 +6204,17 @@
         <v>3</v>
       </c>
       <c r="C366" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
     </row>
     <row r="368" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A368" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
     </row>
     <row r="369" spans="1:3" x14ac:dyDescent="0.3">
       <c r="B369" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
     </row>
     <row r="370" spans="1:3" x14ac:dyDescent="0.3">
@@ -6110,17 +6222,17 @@
         <v>1</v>
       </c>
       <c r="C370" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
     </row>
     <row r="372" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A372" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
     </row>
     <row r="373" spans="1:3" x14ac:dyDescent="0.3">
       <c r="B373" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
     </row>
     <row r="374" spans="1:3" x14ac:dyDescent="0.3">
@@ -6128,7 +6240,7 @@
         <v>1</v>
       </c>
       <c r="C374" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
     </row>
     <row r="375" spans="1:3" x14ac:dyDescent="0.3">
@@ -6136,12 +6248,12 @@
         <v>2</v>
       </c>
       <c r="C375" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
     </row>
     <row r="376" spans="1:3" x14ac:dyDescent="0.3">
       <c r="B376" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
     </row>
     <row r="377" spans="1:3" x14ac:dyDescent="0.3">
@@ -6149,7 +6261,7 @@
         <v>1</v>
       </c>
       <c r="C377" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
     </row>
     <row r="378" spans="1:3" x14ac:dyDescent="0.3">
@@ -6157,7 +6269,7 @@
         <v>2</v>
       </c>
       <c r="C378" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
     </row>
     <row r="379" spans="1:3" x14ac:dyDescent="0.3">
@@ -6165,7 +6277,7 @@
         <v>3</v>
       </c>
       <c r="C379" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
     </row>
     <row r="380" spans="1:3" x14ac:dyDescent="0.3">
@@ -6173,17 +6285,17 @@
         <v>4</v>
       </c>
       <c r="C380" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
     </row>
     <row r="382" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A382" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
     </row>
     <row r="383" spans="1:3" x14ac:dyDescent="0.3">
       <c r="B383" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
     </row>
     <row r="384" spans="1:3" x14ac:dyDescent="0.3">
@@ -6191,12 +6303,12 @@
         <v>1</v>
       </c>
       <c r="C384" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
     </row>
     <row r="385" spans="1:4" x14ac:dyDescent="0.3">
       <c r="B385" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
     </row>
     <row r="386" spans="1:4" x14ac:dyDescent="0.3">
@@ -6204,7 +6316,7 @@
         <v>1</v>
       </c>
       <c r="C386" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
     </row>
     <row r="387" spans="1:4" x14ac:dyDescent="0.3">
@@ -6212,7 +6324,7 @@
         <v>2</v>
       </c>
       <c r="C387" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
     </row>
     <row r="388" spans="1:4" x14ac:dyDescent="0.3">
@@ -6220,23 +6332,23 @@
         <v>3</v>
       </c>
       <c r="C388" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
     </row>
     <row r="390" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A390" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="D390" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
     </row>
     <row r="391" spans="1:4" x14ac:dyDescent="0.3">
       <c r="B391" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="D391" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
     </row>
     <row r="392" spans="1:4" x14ac:dyDescent="0.3">
@@ -6244,26 +6356,26 @@
         <v>1</v>
       </c>
       <c r="C392" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="D392" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
     </row>
     <row r="394" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A394" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="D394" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
     </row>
     <row r="395" spans="1:4" x14ac:dyDescent="0.3">
       <c r="B395" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="D395" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
     </row>
     <row r="396" spans="1:4" x14ac:dyDescent="0.3">
@@ -6271,10 +6383,10 @@
         <v>1</v>
       </c>
       <c r="C396" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="D396" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
     </row>
     <row r="397" spans="1:4" x14ac:dyDescent="0.3">
@@ -6282,7 +6394,7 @@
         <v>2</v>
       </c>
       <c r="C397" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
     </row>
     <row r="398" spans="1:4" x14ac:dyDescent="0.3">
@@ -6290,7 +6402,7 @@
         <v>3</v>
       </c>
       <c r="C398" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
     </row>
     <row r="399" spans="1:4" x14ac:dyDescent="0.3">
@@ -6298,22 +6410,22 @@
         <v>4</v>
       </c>
       <c r="C399" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
     </row>
     <row r="400" spans="1:4" x14ac:dyDescent="0.3">
       <c r="C400" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
     </row>
     <row r="401" spans="1:4" x14ac:dyDescent="0.3">
       <c r="C401" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
     </row>
     <row r="402" spans="1:4" x14ac:dyDescent="0.3">
       <c r="C402" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
     </row>
     <row r="403" spans="1:4" x14ac:dyDescent="0.3">
@@ -6321,17 +6433,17 @@
         <v>5</v>
       </c>
       <c r="C403" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
     </row>
     <row r="408" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A408" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
     </row>
     <row r="409" spans="1:4" x14ac:dyDescent="0.3">
       <c r="B409" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
     </row>
     <row r="410" spans="1:4" x14ac:dyDescent="0.3">
@@ -6339,7 +6451,7 @@
         <v>1</v>
       </c>
       <c r="C410" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
     </row>
     <row r="411" spans="1:4" x14ac:dyDescent="0.3">
@@ -6347,15 +6459,15 @@
         <v>2</v>
       </c>
       <c r="C411" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
     </row>
     <row r="412" spans="1:4" x14ac:dyDescent="0.3">
       <c r="B412" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="D412" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
     </row>
     <row r="413" spans="1:4" x14ac:dyDescent="0.3">
@@ -6363,7 +6475,7 @@
         <v>1</v>
       </c>
       <c r="C413" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
     </row>
     <row r="414" spans="1:4" x14ac:dyDescent="0.3">
@@ -6371,7 +6483,7 @@
         <v>2</v>
       </c>
       <c r="C414" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
     </row>
     <row r="415" spans="1:4" x14ac:dyDescent="0.3">
@@ -6379,10 +6491,10 @@
         <v>3</v>
       </c>
       <c r="C415" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="D415" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
     </row>
     <row r="416" spans="1:4" x14ac:dyDescent="0.3">
@@ -6390,20 +6502,20 @@
         <v>4</v>
       </c>
       <c r="C416" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
     </row>
     <row r="418" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A418" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="D418" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
     </row>
     <row r="419" spans="1:4" x14ac:dyDescent="0.3">
       <c r="B419" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
     </row>
     <row r="420" spans="1:4" x14ac:dyDescent="0.3">
@@ -6411,7 +6523,7 @@
         <v>1</v>
       </c>
       <c r="C420" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
     </row>
     <row r="421" spans="1:4" x14ac:dyDescent="0.3">
@@ -6419,12 +6531,12 @@
         <v>2</v>
       </c>
       <c r="C421" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
     </row>
     <row r="422" spans="1:4" x14ac:dyDescent="0.3">
       <c r="D422" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
     </row>
     <row r="423" spans="1:4" x14ac:dyDescent="0.3">
@@ -6432,7 +6544,7 @@
         <v>3</v>
       </c>
       <c r="C423" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
     </row>
     <row r="424" spans="1:4" x14ac:dyDescent="0.3">
@@ -6440,12 +6552,12 @@
         <v>4</v>
       </c>
       <c r="C424" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
     </row>
     <row r="425" spans="1:4" x14ac:dyDescent="0.3">
       <c r="D425" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
     </row>
     <row r="426" spans="1:4" x14ac:dyDescent="0.3">
@@ -6453,7 +6565,7 @@
         <v>5</v>
       </c>
       <c r="C426" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
     </row>
     <row r="427" spans="1:4" x14ac:dyDescent="0.3">
@@ -6461,7 +6573,7 @@
         <v>6</v>
       </c>
       <c r="C427" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
     </row>
     <row r="429" spans="1:4" x14ac:dyDescent="0.3">
@@ -6469,7 +6581,7 @@
         <v>7</v>
       </c>
       <c r="C429" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
     </row>
     <row r="430" spans="1:4" x14ac:dyDescent="0.3">
@@ -6477,7 +6589,7 @@
         <v>8</v>
       </c>
       <c r="C430" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
     </row>
     <row r="431" spans="1:4" x14ac:dyDescent="0.3">
@@ -6485,7 +6597,7 @@
         <v>9</v>
       </c>
       <c r="C431" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
     </row>
     <row r="433" spans="1:4" x14ac:dyDescent="0.3">
@@ -6493,7 +6605,7 @@
         <v>10</v>
       </c>
       <c r="C433" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
     </row>
     <row r="434" spans="1:4" x14ac:dyDescent="0.3">
@@ -6501,15 +6613,15 @@
         <v>11</v>
       </c>
       <c r="C434" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="D434" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
     </row>
     <row r="436" spans="1:4" x14ac:dyDescent="0.3">
       <c r="B436" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
     </row>
     <row r="437" spans="1:4" x14ac:dyDescent="0.3">
@@ -6517,7 +6629,7 @@
         <v>1</v>
       </c>
       <c r="C437" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
     </row>
     <row r="438" spans="1:4" x14ac:dyDescent="0.3">
@@ -6525,7 +6637,7 @@
         <v>2</v>
       </c>
       <c r="C438" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
     </row>
     <row r="439" spans="1:4" x14ac:dyDescent="0.3">
@@ -6533,7 +6645,7 @@
         <v>3</v>
       </c>
       <c r="C439" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
     </row>
     <row r="440" spans="1:4" x14ac:dyDescent="0.3">
@@ -6541,7 +6653,7 @@
         <v>4</v>
       </c>
       <c r="C440" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
     </row>
     <row r="441" spans="1:4" x14ac:dyDescent="0.3">
@@ -6549,7 +6661,7 @@
         <v>5</v>
       </c>
       <c r="C441" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
     </row>
     <row r="442" spans="1:4" x14ac:dyDescent="0.3">
@@ -6557,7 +6669,7 @@
         <v>6</v>
       </c>
       <c r="C442" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
     </row>
     <row r="443" spans="1:4" x14ac:dyDescent="0.3">
@@ -6565,17 +6677,17 @@
         <v>7</v>
       </c>
       <c r="C443" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
     </row>
     <row r="446" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A446" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
     </row>
     <row r="447" spans="1:4" x14ac:dyDescent="0.3">
       <c r="B447" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
     </row>
   </sheetData>
@@ -6602,291 +6714,291 @@
   <sheetData>
     <row r="1" spans="1:3" ht="18" x14ac:dyDescent="0.35">
       <c r="A1" s="16" t="s">
-        <v>475</v>
+        <v>474</v>
       </c>
     </row>
     <row r="2" spans="1:3" ht="18" x14ac:dyDescent="0.35">
       <c r="A2" s="16" t="s">
-        <v>474</v>
+        <v>473</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A4" s="11" t="s">
-        <v>357</v>
+        <v>356</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A5" s="11" t="s">
-        <v>358</v>
+        <v>357</v>
       </c>
       <c r="B5" s="11" t="s">
-        <v>347</v>
+        <v>346</v>
       </c>
       <c r="C5" s="11" t="s">
-        <v>329</v>
+        <v>328</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.3">
       <c r="B6" s="12" t="s">
-        <v>330</v>
+        <v>329</v>
       </c>
       <c r="C6" s="11" t="s">
-        <v>359</v>
+        <v>358</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.3">
       <c r="B7" s="12" t="s">
-        <v>332</v>
+        <v>331</v>
       </c>
       <c r="C7" s="11" t="s">
-        <v>360</v>
+        <v>359</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.3">
       <c r="B8" s="12" t="s">
-        <v>336</v>
+        <v>335</v>
       </c>
       <c r="C8" s="11" t="s">
-        <v>361</v>
+        <v>360</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.3">
       <c r="B9" s="12" t="s">
-        <v>338</v>
+        <v>337</v>
       </c>
       <c r="C9" s="13" t="s">
-        <v>362</v>
+        <v>361</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.3">
       <c r="B10" s="12" t="s">
-        <v>340</v>
+        <v>339</v>
       </c>
       <c r="C10" s="11" t="s">
-        <v>363</v>
+        <v>362</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.3">
       <c r="B11" s="12" t="s">
+        <v>363</v>
+      </c>
+      <c r="C11" s="13" t="s">
         <v>364</v>
-      </c>
-      <c r="C11" s="13" t="s">
-        <v>365</v>
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A12" s="11" t="s">
+        <v>365</v>
+      </c>
+      <c r="B12" s="11" t="s">
         <v>366</v>
       </c>
-      <c r="B12" s="11" t="s">
-        <v>367</v>
-      </c>
       <c r="C12" s="11" t="s">
-        <v>329</v>
+        <v>328</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.3">
       <c r="B13" s="12" t="s">
-        <v>330</v>
+        <v>329</v>
       </c>
       <c r="C13" s="11" t="s">
-        <v>359</v>
+        <v>358</v>
       </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.3">
       <c r="B14" s="12" t="s">
-        <v>332</v>
+        <v>331</v>
       </c>
       <c r="C14" s="11" t="s">
-        <v>360</v>
+        <v>359</v>
       </c>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.3">
       <c r="B15" s="12" t="s">
-        <v>336</v>
+        <v>335</v>
       </c>
       <c r="C15" s="11" t="s">
-        <v>361</v>
+        <v>360</v>
       </c>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.3">
       <c r="B16" s="12" t="s">
-        <v>338</v>
+        <v>337</v>
       </c>
       <c r="C16" s="11" t="s">
-        <v>368</v>
+        <v>367</v>
       </c>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A18" s="11" t="s">
-        <v>324</v>
+        <v>323</v>
       </c>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A19" s="11" t="s">
+        <v>326</v>
+      </c>
+      <c r="B19" s="11" t="s">
         <v>327</v>
       </c>
-      <c r="B19" s="11" t="s">
+      <c r="C19" s="11" t="s">
         <v>328</v>
-      </c>
-      <c r="C19" s="11" t="s">
-        <v>329</v>
       </c>
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.3">
       <c r="B20" s="12" t="s">
+        <v>329</v>
+      </c>
+      <c r="C20" s="11" t="s">
         <v>330</v>
-      </c>
-      <c r="C20" s="11" t="s">
-        <v>331</v>
       </c>
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.3">
       <c r="B21" s="12" t="s">
+        <v>331</v>
+      </c>
+      <c r="C21" s="11" t="s">
         <v>332</v>
-      </c>
-      <c r="C21" s="11" t="s">
-        <v>333</v>
       </c>
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.3">
       <c r="C22" s="11" t="s">
-        <v>334</v>
+        <v>333</v>
       </c>
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.3">
       <c r="C23" s="11" t="s">
-        <v>335</v>
+        <v>334</v>
       </c>
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.3">
       <c r="B24" s="12" t="s">
+        <v>335</v>
+      </c>
+      <c r="C24" s="11" t="s">
         <v>336</v>
-      </c>
-      <c r="C24" s="11" t="s">
-        <v>337</v>
       </c>
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.3">
       <c r="B25" s="12" t="s">
+        <v>337</v>
+      </c>
+      <c r="C25" s="13" t="s">
         <v>338</v>
-      </c>
-      <c r="C25" s="13" t="s">
-        <v>339</v>
       </c>
     </row>
     <row r="26" spans="1:3" x14ac:dyDescent="0.3">
       <c r="B26" s="12" t="s">
+        <v>339</v>
+      </c>
+      <c r="C26" s="13" t="s">
         <v>340</v>
-      </c>
-      <c r="C26" s="13" t="s">
-        <v>341</v>
       </c>
     </row>
     <row r="27" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A27" s="11" t="s">
+        <v>341</v>
+      </c>
+      <c r="B27" s="11" t="s">
         <v>342</v>
       </c>
-      <c r="B27" s="11" t="s">
-        <v>343</v>
-      </c>
       <c r="C27" s="11" t="s">
-        <v>329</v>
+        <v>328</v>
       </c>
     </row>
     <row r="28" spans="1:3" x14ac:dyDescent="0.3">
       <c r="B28" s="12" t="s">
-        <v>330</v>
+        <v>329</v>
       </c>
       <c r="C28" s="11" t="s">
-        <v>344</v>
+        <v>343</v>
       </c>
     </row>
     <row r="29" spans="1:3" x14ac:dyDescent="0.3">
       <c r="B29" s="12" t="s">
-        <v>332</v>
+        <v>331</v>
       </c>
       <c r="C29" s="11" t="s">
-        <v>345</v>
+        <v>344</v>
       </c>
     </row>
     <row r="30" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A30" s="11" t="s">
+        <v>345</v>
+      </c>
+      <c r="B30" s="11" t="s">
         <v>346</v>
       </c>
-      <c r="B30" s="11" t="s">
-        <v>347</v>
-      </c>
       <c r="C30" s="11" t="s">
-        <v>329</v>
+        <v>328</v>
       </c>
     </row>
     <row r="31" spans="1:3" x14ac:dyDescent="0.3">
       <c r="B31" s="12" t="s">
-        <v>330</v>
+        <v>329</v>
       </c>
       <c r="C31" s="11" t="s">
-        <v>348</v>
+        <v>347</v>
       </c>
     </row>
     <row r="32" spans="1:3" x14ac:dyDescent="0.3">
       <c r="C32" s="11" t="s">
-        <v>349</v>
+        <v>348</v>
       </c>
     </row>
     <row r="33" spans="1:3" x14ac:dyDescent="0.3">
       <c r="B33" s="12" t="s">
-        <v>332</v>
+        <v>331</v>
       </c>
       <c r="C33" s="13" t="s">
-        <v>350</v>
+        <v>349</v>
       </c>
     </row>
     <row r="34" spans="1:3" x14ac:dyDescent="0.3">
       <c r="B34" s="12" t="s">
-        <v>336</v>
+        <v>335</v>
       </c>
       <c r="C34" s="13" t="s">
-        <v>351</v>
+        <v>350</v>
       </c>
     </row>
     <row r="35" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A35" s="11" t="s">
+        <v>351</v>
+      </c>
+      <c r="B35" s="11" t="s">
         <v>352</v>
       </c>
-      <c r="B35" s="11" t="s">
-        <v>353</v>
-      </c>
       <c r="C35" s="11" t="s">
-        <v>329</v>
+        <v>328</v>
       </c>
     </row>
     <row r="36" spans="1:3" x14ac:dyDescent="0.3">
       <c r="B36" s="11" t="s">
-        <v>328</v>
+        <v>327</v>
       </c>
     </row>
     <row r="37" spans="1:3" x14ac:dyDescent="0.3">
       <c r="B37" s="11" t="s">
-        <v>347</v>
+        <v>346</v>
       </c>
     </row>
     <row r="38" spans="1:3" x14ac:dyDescent="0.3">
       <c r="B38" s="12" t="s">
-        <v>330</v>
+        <v>329</v>
       </c>
       <c r="C38" s="11" t="s">
-        <v>354</v>
+        <v>353</v>
       </c>
     </row>
     <row r="39" spans="1:3" x14ac:dyDescent="0.3">
       <c r="C39" s="11" t="s">
-        <v>355</v>
+        <v>354</v>
       </c>
     </row>
     <row r="40" spans="1:3" x14ac:dyDescent="0.3">
       <c r="C40" s="13" t="s">
-        <v>356</v>
+        <v>355</v>
       </c>
     </row>
   </sheetData>

</xml_diff>